<commit_message>
Intensity check for isotopes start
</commit_message>
<xml_diff>
--- a/dev/isotopes.xlsx
+++ b/dev/isotopes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo Cunha\Documents\GitHub\streamFind\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{67603D8D-FE3E-4022-B7FC-21E5DA745F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72A8462-B3DA-467C-8236-673B01837904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-12540" windowWidth="29040" windowHeight="18240" activeTab="1"/>
+    <workbookView xWindow="-57720" yWindow="-12540" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
   <si>
     <t>element</t>
   </si>
@@ -340,11 +351,29 @@
   <si>
     <t>U</t>
   </si>
+  <si>
+    <t>M+1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>rel</t>
+  </si>
+  <si>
+    <t>O18</t>
+  </si>
+  <si>
+    <t>Cl37</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1178,11 +1207,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6973,16 +7002,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AC85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AA60" sqref="AA60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>isotopes!A1</f>
         <v>element</v>
@@ -7052,7 +7084,7 @@
         <v>i7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>isotopes!A2</f>
         <v>H</v>
@@ -7066,23 +7098,23 @@
         <v>1.007825032</v>
       </c>
       <c r="D2">
-        <f>isotopes!D2</f>
-        <v>99.984425999999999</v>
+        <f>isotopes!D2/100</f>
+        <v>0.99984426000000004</v>
       </c>
       <c r="E2">
         <f>IF(isotopes!E2-C2&lt;0,0,isotopes!E2-C2)</f>
         <v>1.0062767460000002</v>
       </c>
       <c r="F2">
-        <f>isotopes!F2</f>
-        <v>1.5573999999999999E-2</v>
+        <f>isotopes!F2/100</f>
+        <v>1.5574E-4</v>
       </c>
       <c r="G2">
         <f>IF(isotopes!G2-C2&lt;0,0,isotopes!G2-C2)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>isotopes!H2</f>
+        <f>isotopes!H2/100</f>
         <v>0</v>
       </c>
       <c r="I2">
@@ -7122,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>isotopes!A3</f>
         <v>He</v>
@@ -7136,23 +7168,23 @@
         <v>3.01602931</v>
       </c>
       <c r="D3">
-        <f>isotopes!D3</f>
-        <v>1.3430000000000001E-4</v>
+        <f>isotopes!D3/100</f>
+        <v>1.3430000000000001E-6</v>
       </c>
       <c r="E3">
         <f>IF(isotopes!E3-C3&lt;0,0,isotopes!E3-C3)</f>
         <v>0.98657393999999998</v>
       </c>
       <c r="F3">
-        <f>isotopes!F3</f>
-        <v>99.999865700000001</v>
+        <f>isotopes!F3/100</f>
+        <v>0.99999865700000001</v>
       </c>
       <c r="G3">
         <f>IF(isotopes!G3-C3&lt;0,0,isotopes!G3-C3)</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>isotopes!H3</f>
+        <f>isotopes!H3/100</f>
         <v>0</v>
       </c>
       <c r="I3">
@@ -7192,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>isotopes!A4</f>
         <v>Li</v>
@@ -7206,23 +7238,23 @@
         <v>6.0151222999999998</v>
       </c>
       <c r="D4">
-        <f>isotopes!D4</f>
-        <v>7.5890000000000004</v>
+        <f>isotopes!D4/100</f>
+        <v>7.5889999999999999E-2</v>
       </c>
       <c r="E4">
         <f>IF(isotopes!E4-C4&lt;0,0,isotopes!E4-C4)</f>
         <v>1.0008816999999999</v>
       </c>
       <c r="F4">
-        <f>isotopes!F4</f>
-        <v>92.411000000000001</v>
+        <f>isotopes!F4/100</f>
+        <v>0.92410999999999999</v>
       </c>
       <c r="G4">
         <f>IF(isotopes!G4-C4&lt;0,0,isotopes!G4-C4)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>isotopes!H4</f>
+        <f>isotopes!H4/100</f>
         <v>0</v>
       </c>
       <c r="I4">
@@ -7262,7 +7294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>isotopes!A5</f>
         <v>Be</v>
@@ -7276,15 +7308,15 @@
         <v>9.0121821000000004</v>
       </c>
       <c r="D5">
-        <f>isotopes!D5</f>
-        <v>100</v>
+        <f>isotopes!D5/100</f>
+        <v>1</v>
       </c>
       <c r="E5">
         <f>IF(isotopes!E5-C5&lt;0,0,isotopes!E5-C5)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>isotopes!F5</f>
+        <f>isotopes!F5/100</f>
         <v>0</v>
       </c>
       <c r="G5">
@@ -7292,7 +7324,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <f>isotopes!H5</f>
+        <f>isotopes!H5/100</f>
         <v>0</v>
       </c>
       <c r="I5">
@@ -7332,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>isotopes!A6</f>
         <v>B</v>
@@ -7346,23 +7378,23 @@
         <v>10.012937000000001</v>
       </c>
       <c r="D6">
-        <f>isotopes!D6</f>
-        <v>19.82</v>
+        <f>isotopes!D6/100</f>
+        <v>0.19820000000000002</v>
       </c>
       <c r="E6">
         <f>IF(isotopes!E6-C6&lt;0,0,isotopes!E6-C6)</f>
         <v>0.9963684999999991</v>
       </c>
       <c r="F6">
-        <f>isotopes!F6</f>
-        <v>80.180000000000007</v>
+        <f>isotopes!F6/100</f>
+        <v>0.80180000000000007</v>
       </c>
       <c r="G6">
         <f>IF(isotopes!G6-C6&lt;0,0,isotopes!G6-C6)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>isotopes!H6</f>
+        <f>isotopes!H6/100</f>
         <v>0</v>
       </c>
       <c r="I6">
@@ -7401,8 +7433,15 @@
         <f>isotopes!Q6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>106</v>
+      </c>
+      <c r="W6">
+        <f>W10*W8*W7</f>
+        <v>61.361041999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>isotopes!A7</f>
         <v>C</v>
@@ -7416,23 +7455,23 @@
         <v>12</v>
       </c>
       <c r="D7">
-        <f>isotopes!D7</f>
-        <v>98.892200000000003</v>
+        <f>isotopes!D7/100</f>
+        <v>0.98892200000000008</v>
       </c>
       <c r="E7">
         <f>IF(isotopes!E7-C7&lt;0,0,isotopes!E7-C7)</f>
         <v>1.0033548400000001</v>
       </c>
       <c r="F7">
-        <f>isotopes!F7</f>
-        <v>1.1077999999999999</v>
+        <f>isotopes!F7/100</f>
+        <v>1.1077999999999999E-2</v>
       </c>
       <c r="G7">
         <f>IF(isotopes!G7-C7&lt;0,0,isotopes!G7-C7)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>isotopes!H7</f>
+        <f>isotopes!H7/100</f>
         <v>0</v>
       </c>
       <c r="I7">
@@ -7471,8 +7510,14 @@
         <f>isotopes!Q7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>107</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>isotopes!A8</f>
         <v>N</v>
@@ -7486,23 +7531,23 @@
         <v>14.003074010000001</v>
       </c>
       <c r="D8">
-        <f>isotopes!D8</f>
-        <v>99.633700000000005</v>
+        <f>isotopes!D8/100</f>
+        <v>0.99633700000000003</v>
       </c>
       <c r="E8">
         <f>IF(isotopes!E8-C8&lt;0,0,isotopes!E8-C8)</f>
         <v>0.99703489000000012</v>
       </c>
       <c r="F8">
-        <f>isotopes!F8</f>
-        <v>0.36630000000000001</v>
+        <f>isotopes!F8/100</f>
+        <v>3.663E-3</v>
       </c>
       <c r="G8">
         <f>IF(isotopes!G8-C8&lt;0,0,isotopes!G8-C8)</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>isotopes!H8</f>
+        <f>isotopes!H8/100</f>
         <v>0</v>
       </c>
       <c r="I8">
@@ -7541,8 +7586,15 @@
         <f>isotopes!Q8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>108</v>
+      </c>
+      <c r="W8">
+        <f>((F7*F7)/2)*100</f>
+        <v>6.1361041999999991E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>isotopes!A9</f>
         <v>O</v>
@@ -7556,24 +7608,24 @@
         <v>15.994914619999999</v>
       </c>
       <c r="D9">
-        <f>isotopes!D9</f>
-        <v>99.762799999999999</v>
+        <f>isotopes!D9/100</f>
+        <v>0.99762799999999996</v>
       </c>
       <c r="E9">
         <f>IF(isotopes!E9-C9&lt;0,0,isotopes!E9-C9)</f>
         <v>1.0042168800000013</v>
       </c>
       <c r="F9">
-        <f>isotopes!F9</f>
-        <v>3.7199999999999997E-2</v>
+        <f>isotopes!F9/100</f>
+        <v>3.7199999999999999E-4</v>
       </c>
       <c r="G9">
         <f>IF(isotopes!G9-C9&lt;0,0,isotopes!G9-C9)</f>
         <v>2.0042457800000015</v>
       </c>
       <c r="H9">
-        <f>isotopes!H9</f>
-        <v>0.20004</v>
+        <f>isotopes!H9/100</f>
+        <v>2.0003999999999998E-3</v>
       </c>
       <c r="I9">
         <f>isotopes!I9</f>
@@ -7612,7 +7664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>isotopes!A10</f>
         <v>F</v>
@@ -7626,15 +7678,15 @@
         <v>18.998403199999998</v>
       </c>
       <c r="D10">
-        <f>isotopes!D10</f>
-        <v>100</v>
+        <f>isotopes!D10/100</f>
+        <v>1</v>
       </c>
       <c r="E10">
         <f>IF(isotopes!E10-C10&lt;0,0,isotopes!E10-C10)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>isotopes!F10</f>
+        <f>isotopes!F10/100</f>
         <v>0</v>
       </c>
       <c r="G10">
@@ -7642,7 +7694,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <f>isotopes!H10</f>
+        <f>isotopes!H10/100</f>
         <v>0</v>
       </c>
       <c r="I10">
@@ -7681,8 +7733,14 @@
         <f>isotopes!Q10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>111</v>
+      </c>
+      <c r="W10">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>isotopes!A11</f>
         <v>Ne</v>
@@ -7696,24 +7754,24 @@
         <v>19.992440179999999</v>
       </c>
       <c r="D11">
-        <f>isotopes!D11</f>
-        <v>90.483800000000002</v>
+        <f>isotopes!D11/100</f>
+        <v>0.90483800000000003</v>
       </c>
       <c r="E11">
         <f>IF(isotopes!E11-C11&lt;0,0,isotopes!E11-C11)</f>
         <v>1.0014065599999995</v>
       </c>
       <c r="F11">
-        <f>isotopes!F11</f>
-        <v>0.26960000000000001</v>
+        <f>isotopes!F11/100</f>
+        <v>2.696E-3</v>
       </c>
       <c r="G11">
         <f>IF(isotopes!G11-C11&lt;0,0,isotopes!G11-C11)</f>
         <v>1.9989453300000015</v>
       </c>
       <c r="H11">
-        <f>isotopes!H11</f>
-        <v>9.2464999999999993</v>
+        <f>isotopes!H11/100</f>
+        <v>9.2464999999999992E-2</v>
       </c>
       <c r="I11">
         <f>isotopes!I11</f>
@@ -7752,7 +7810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>isotopes!A12</f>
         <v>Na</v>
@@ -7766,15 +7824,15 @@
         <v>22.989769670000001</v>
       </c>
       <c r="D12">
-        <f>isotopes!D12</f>
-        <v>100</v>
+        <f>isotopes!D12/100</f>
+        <v>1</v>
       </c>
       <c r="E12">
         <f>IF(isotopes!E12-C12&lt;0,0,isotopes!E12-C12)</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>isotopes!F12</f>
+        <f>isotopes!F12/100</f>
         <v>0</v>
       </c>
       <c r="G12">
@@ -7782,7 +7840,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <f>isotopes!H12</f>
+        <f>isotopes!H12/100</f>
         <v>0</v>
       </c>
       <c r="I12">
@@ -7822,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>isotopes!A13</f>
         <v>Mg</v>
@@ -7836,24 +7894,24 @@
         <v>23.985041899999999</v>
       </c>
       <c r="D13">
-        <f>isotopes!D13</f>
-        <v>78.992000000000004</v>
+        <f>isotopes!D13/100</f>
+        <v>0.78992000000000007</v>
       </c>
       <c r="E13">
         <f>IF(isotopes!E13-C13&lt;0,0,isotopes!E13-C13)</f>
         <v>1.0007951200000029</v>
       </c>
       <c r="F13">
-        <f>isotopes!F13</f>
-        <v>10.003</v>
+        <f>isotopes!F13/100</f>
+        <v>0.10003000000000001</v>
       </c>
       <c r="G13">
         <f>IF(isotopes!G13-C13&lt;0,0,isotopes!G13-C13)</f>
         <v>1.9975511400000023</v>
       </c>
       <c r="H13">
-        <f>isotopes!H13</f>
-        <v>11.005000000000001</v>
+        <f>isotopes!H13/100</f>
+        <v>0.11005000000000001</v>
       </c>
       <c r="I13">
         <f>isotopes!I13</f>
@@ -7891,8 +7949,27 @@
         <f>isotopes!Q13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V13" t="s">
+        <v>106</v>
+      </c>
+      <c r="W13">
+        <f>W17*W15*W14</f>
+        <v>0.66467999999999994</v>
+      </c>
+      <c r="Y13">
+        <f>Y17*Y15*Y14</f>
+        <v>0.48458000000000001</v>
+      </c>
+      <c r="AA13">
+        <f>AA17*AA15*AA14</f>
+        <v>2.8033199999999998E-3</v>
+      </c>
+      <c r="AC13">
+        <f>AC17*AC15*AC14</f>
+        <v>3.6007199999999996E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>isotopes!A14</f>
         <v>Al</v>
@@ -7906,15 +7983,15 @@
         <v>26.981538440000001</v>
       </c>
       <c r="D14">
-        <f>isotopes!D14</f>
-        <v>100</v>
+        <f>isotopes!D14/100</f>
+        <v>1</v>
       </c>
       <c r="E14">
         <f>IF(isotopes!E14-C14&lt;0,0,isotopes!E14-C14)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>isotopes!F14</f>
+        <f>isotopes!F14/100</f>
         <v>0</v>
       </c>
       <c r="G14">
@@ -7922,7 +7999,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <f>isotopes!H14</f>
+        <f>isotopes!H14/100</f>
         <v>0</v>
       </c>
       <c r="I14">
@@ -7961,8 +8038,23 @@
         <f>isotopes!Q14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
+        <v>107</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>isotopes!A15</f>
         <v>Si</v>
@@ -7976,24 +8068,24 @@
         <v>27.97692653</v>
       </c>
       <c r="D15">
-        <f>isotopes!D15</f>
-        <v>92.229680000000002</v>
+        <f>isotopes!D15/100</f>
+        <v>0.92229680000000003</v>
       </c>
       <c r="E15">
         <f>IF(isotopes!E15-C15&lt;0,0,isotopes!E15-C15)</f>
         <v>0.99956819000000152</v>
       </c>
       <c r="F15">
-        <f>isotopes!F15</f>
-        <v>4.68316</v>
+        <f>isotopes!F15/100</f>
+        <v>4.6831600000000001E-2</v>
       </c>
       <c r="G15">
         <f>IF(isotopes!G15-C15&lt;0,0,isotopes!G15-C15)</f>
         <v>1.9968436899999986</v>
       </c>
       <c r="H15">
-        <f>isotopes!H15</f>
-        <v>3.0871599999999999</v>
+        <f>isotopes!H15/100</f>
+        <v>3.0871599999999999E-2</v>
       </c>
       <c r="I15">
         <f>isotopes!I15</f>
@@ -8031,8 +8123,27 @@
         <f>isotopes!Q15</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>108</v>
+      </c>
+      <c r="W15">
+        <f>F7</f>
+        <v>1.1077999999999999E-2</v>
+      </c>
+      <c r="Y15">
+        <f>F18</f>
+        <v>0.24229000000000001</v>
+      </c>
+      <c r="AA15">
+        <f>F2</f>
+        <v>1.5574E-4</v>
+      </c>
+      <c r="AC15">
+        <f>H9</f>
+        <v>2.0003999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>isotopes!A16</f>
         <v>P</v>
@@ -8046,15 +8157,15 @@
         <v>30.973761509999999</v>
       </c>
       <c r="D16">
-        <f>isotopes!D16</f>
-        <v>100</v>
+        <f>isotopes!D16/100</f>
+        <v>1</v>
       </c>
       <c r="E16">
         <f>IF(isotopes!E16-C16&lt;0,0,isotopes!E16-C16)</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>isotopes!F16</f>
+        <f>isotopes!F16/100</f>
         <v>0</v>
       </c>
       <c r="G16">
@@ -8062,7 +8173,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <f>isotopes!H16</f>
+        <f>isotopes!H16/100</f>
         <v>0</v>
       </c>
       <c r="I16">
@@ -8102,7 +8213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>isotopes!A17</f>
         <v>S</v>
@@ -8116,24 +8227,24 @@
         <v>31.972070689999999</v>
       </c>
       <c r="D17">
-        <f>isotopes!D17</f>
-        <v>95.018000000000001</v>
+        <f>isotopes!D17/100</f>
+        <v>0.95018000000000002</v>
       </c>
       <c r="E17">
         <f>IF(isotopes!E17-C17&lt;0,0,isotopes!E17-C17)</f>
         <v>0.99938780999999821</v>
       </c>
       <c r="F17">
-        <f>isotopes!F17</f>
-        <v>0.75</v>
+        <f>isotopes!F17/100</f>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="G17">
         <f>IF(isotopes!G17-C17&lt;0,0,isotopes!G17-C17)</f>
         <v>1.9957961399999995</v>
       </c>
       <c r="H17">
-        <f>isotopes!H17</f>
-        <v>4.2149999999999999</v>
+        <f>isotopes!H17/100</f>
+        <v>4.215E-2</v>
       </c>
       <c r="I17">
         <f>isotopes!I17</f>
@@ -8171,8 +8282,32 @@
         <f>isotopes!Q17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>111</v>
+      </c>
+      <c r="W17">
+        <v>60</v>
+      </c>
+      <c r="X17" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y17">
+        <v>2</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA17">
+        <v>18</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>isotopes!A18</f>
         <v>Cl</v>
@@ -8186,23 +8321,23 @@
         <v>34.96885271</v>
       </c>
       <c r="D18">
-        <f>isotopes!D18</f>
-        <v>75.771000000000001</v>
+        <f>isotopes!D18/100</f>
+        <v>0.75770999999999999</v>
       </c>
       <c r="E18">
         <f>IF(isotopes!E18-C18&lt;0,0,isotopes!E18-C18)</f>
         <v>1.9970498899999996</v>
       </c>
       <c r="F18">
-        <f>isotopes!F18</f>
-        <v>24.228999999999999</v>
+        <f>isotopes!F18/100</f>
+        <v>0.24229000000000001</v>
       </c>
       <c r="G18">
         <f>IF(isotopes!G18-C18&lt;0,0,isotopes!G18-C18)</f>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>isotopes!H18</f>
+        <f>isotopes!H18/100</f>
         <v>0</v>
       </c>
       <c r="I18">
@@ -8242,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>isotopes!A19</f>
         <v>Ar</v>
@@ -8256,24 +8391,24 @@
         <v>35.967546280000001</v>
       </c>
       <c r="D19">
-        <f>isotopes!D19</f>
-        <v>0.33650000000000002</v>
+        <f>isotopes!D19/100</f>
+        <v>3.3650000000000004E-3</v>
       </c>
       <c r="E19">
         <f>IF(isotopes!E19-C19&lt;0,0,isotopes!E19-C19)</f>
         <v>1.9951859199999973</v>
       </c>
       <c r="F19">
-        <f>isotopes!F19</f>
-        <v>6.3200000000000006E-2</v>
+        <f>isotopes!F19/100</f>
+        <v>6.3200000000000007E-4</v>
       </c>
       <c r="G19">
         <f>IF(isotopes!G19-C19&lt;0,0,isotopes!G19-C19)</f>
         <v>3.9948368399999978</v>
       </c>
       <c r="H19">
-        <f>isotopes!H19</f>
-        <v>99.600300000000004</v>
+        <f>isotopes!H19/100</f>
+        <v>0.99600300000000008</v>
       </c>
       <c r="I19">
         <f>isotopes!I19</f>
@@ -8312,7 +8447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>isotopes!A20</f>
         <v>K</v>
@@ -8326,24 +8461,24 @@
         <v>38.963706899999998</v>
       </c>
       <c r="D20">
-        <f>isotopes!D20</f>
-        <v>93.258110000000002</v>
+        <f>isotopes!D20/100</f>
+        <v>0.93258110000000005</v>
       </c>
       <c r="E20">
         <f>IF(isotopes!E20-C20&lt;0,0,isotopes!E20-C20)</f>
         <v>1.000291770000004</v>
       </c>
       <c r="F20">
-        <f>isotopes!F20</f>
-        <v>1.1672E-2</v>
+        <f>isotopes!F20/100</f>
+        <v>1.1672000000000001E-4</v>
       </c>
       <c r="G20">
         <f>IF(isotopes!G20-C20&lt;0,0,isotopes!G20-C20)</f>
         <v>1.9981190700000013</v>
       </c>
       <c r="H20">
-        <f>isotopes!H20</f>
-        <v>6.7302200000000001</v>
+        <f>isotopes!H20/100</f>
+        <v>6.7302200000000006E-2</v>
       </c>
       <c r="I20">
         <f>isotopes!I20</f>
@@ -8381,8 +8516,18 @@
         <f>isotopes!Q20</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V20">
+        <v>195.12270013</v>
+      </c>
+      <c r="X20">
+        <v>100</v>
+      </c>
+      <c r="Y20">
+        <f>X20/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>isotopes!A21</f>
         <v>Ca</v>
@@ -8396,24 +8541,24 @@
         <v>39.962591199999999</v>
       </c>
       <c r="D21">
-        <f>isotopes!D21</f>
-        <v>96.941000000000003</v>
+        <f>isotopes!D21/100</f>
+        <v>0.96940999999999999</v>
       </c>
       <c r="E21">
         <f>IF(isotopes!E21-C21&lt;0,0,isotopes!E21-C21)</f>
         <v>1.9960270999999992</v>
       </c>
       <c r="F21">
-        <f>isotopes!F21</f>
-        <v>0.64700000000000002</v>
+        <f>isotopes!F21/100</f>
+        <v>6.4700000000000001E-3</v>
       </c>
       <c r="G21">
         <f>IF(isotopes!G21-C21&lt;0,0,isotopes!G21-C21)</f>
         <v>2.9961756000000008</v>
       </c>
       <c r="H21">
-        <f>isotopes!H21</f>
-        <v>0.13500000000000001</v>
+        <f>isotopes!H21/100</f>
+        <v>1.3500000000000001E-3</v>
       </c>
       <c r="I21">
         <f>isotopes!I21</f>
@@ -8451,8 +8596,22 @@
         <f>isotopes!Q21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V21">
+        <v>196.1260834</v>
+      </c>
+      <c r="W21">
+        <f>V21-$V$20</f>
+        <v>1.0033832700000005</v>
+      </c>
+      <c r="X21">
+        <v>8.9247630000000004</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" ref="Y21:Y26" si="0">X21/100</f>
+        <v>8.9247630000000008E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>isotopes!A22</f>
         <v>Sc</v>
@@ -8466,15 +8625,15 @@
         <v>44.955910199999998</v>
       </c>
       <c r="D22">
-        <f>isotopes!D22</f>
-        <v>100</v>
+        <f>isotopes!D22/100</f>
+        <v>1</v>
       </c>
       <c r="E22">
         <f>IF(isotopes!E22-C22&lt;0,0,isotopes!E22-C22)</f>
         <v>0</v>
       </c>
       <c r="F22">
-        <f>isotopes!F22</f>
+        <f>isotopes!F22/100</f>
         <v>0</v>
       </c>
       <c r="G22">
@@ -8482,7 +8641,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <f>isotopes!H22</f>
+        <f>isotopes!H22/100</f>
         <v>0</v>
       </c>
       <c r="I22">
@@ -8521,8 +8680,22 @@
         <f>isotopes!Q22</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V22">
+        <v>196.12923598</v>
+      </c>
+      <c r="W22">
+        <f t="shared" ref="W22:W26" si="1">V22-$V$20</f>
+        <v>1.0065358500000059</v>
+      </c>
+      <c r="X22">
+        <v>0.18340799999999999</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="0"/>
+        <v>1.8340799999999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>isotopes!A23</f>
         <v>Ti</v>
@@ -8536,24 +8709,24 @@
         <v>45.9526295</v>
       </c>
       <c r="D23">
-        <f>isotopes!D23</f>
-        <v>8.2490000000000006</v>
+        <f>isotopes!D23/100</f>
+        <v>8.2490000000000008E-2</v>
       </c>
       <c r="E23">
         <f>IF(isotopes!E23-C23&lt;0,0,isotopes!E23-C23)</f>
         <v>0.99913430000000147</v>
       </c>
       <c r="F23">
-        <f>isotopes!F23</f>
-        <v>7.4370000000000003</v>
+        <f>isotopes!F23/100</f>
+        <v>7.4370000000000006E-2</v>
       </c>
       <c r="G23">
         <f>IF(isotopes!G23-C23&lt;0,0,isotopes!G23-C23)</f>
         <v>1.9953175999999999</v>
       </c>
       <c r="H23">
-        <f>isotopes!H23</f>
-        <v>73.72</v>
+        <f>isotopes!H23/100</f>
+        <v>0.73719999999999997</v>
       </c>
       <c r="I23">
         <f>isotopes!I23</f>
@@ -8591,8 +8764,22 @@
         <f>isotopes!Q23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V23">
+        <v>197.12697975</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="1"/>
+        <v>2.0042796200000055</v>
+      </c>
+      <c r="X23">
+        <v>1.0591010000000001</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="0"/>
+        <v>1.0591010000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>isotopes!A24</f>
         <v>V</v>
@@ -8606,23 +8793,23 @@
         <v>49.947162800000001</v>
       </c>
       <c r="D24">
-        <f>isotopes!D24</f>
-        <v>0.24970000000000001</v>
+        <f>isotopes!D24/100</f>
+        <v>2.4970000000000001E-3</v>
       </c>
       <c r="E24">
         <f>IF(isotopes!E24-C24&lt;0,0,isotopes!E24-C24)</f>
         <v>0.99680089999999666</v>
       </c>
       <c r="F24">
-        <f>isotopes!F24</f>
-        <v>99.750299999999996</v>
+        <f>isotopes!F24/100</f>
+        <v>0.99750299999999992</v>
       </c>
       <c r="G24">
         <f>IF(isotopes!G24-C24&lt;0,0,isotopes!G24-C24)</f>
         <v>0</v>
       </c>
       <c r="H24">
-        <f>isotopes!H24</f>
+        <f>isotopes!H24/100</f>
         <v>0</v>
       </c>
       <c r="I24">
@@ -8661,8 +8848,22 @@
         <f>isotopes!Q24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V24">
+        <v>197.12960466000001</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="1"/>
+        <v>2.0069045300000141</v>
+      </c>
+      <c r="X24">
+        <v>0.32888200000000001</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="0"/>
+        <v>3.28882E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>isotopes!A25</f>
         <v>Cr</v>
@@ -8676,24 +8877,24 @@
         <v>49.946049600000002</v>
       </c>
       <c r="D25">
-        <f>isotopes!D25</f>
-        <v>4.3452000000000002</v>
+        <f>isotopes!D25/100</f>
+        <v>4.3452000000000005E-2</v>
       </c>
       <c r="E25">
         <f>IF(isotopes!E25-C25&lt;0,0,isotopes!E25-C25)</f>
         <v>1.994462299999995</v>
       </c>
       <c r="F25">
-        <f>isotopes!F25</f>
-        <v>83.789500000000004</v>
+        <f>isotopes!F25/100</f>
+        <v>0.83789500000000006</v>
       </c>
       <c r="G25">
         <f>IF(isotopes!G25-C25&lt;0,0,isotopes!G25-C25)</f>
         <v>2.9946041999999977</v>
       </c>
       <c r="H25">
-        <f>isotopes!H25</f>
-        <v>9.5006000000000004</v>
+        <f>isotopes!H25/100</f>
+        <v>9.5006000000000007E-2</v>
       </c>
       <c r="I25">
         <f>isotopes!I25</f>
@@ -8731,8 +8932,22 @@
         <f>isotopes!Q25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V25">
+        <v>197.13254617000001</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="1"/>
+        <v>2.0098460400000135</v>
+      </c>
+      <c r="X25">
+        <v>1.6733000000000001E-2</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="0"/>
+        <v>1.6733000000000001E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>isotopes!A26</f>
         <v>Mn</v>
@@ -8746,15 +8961,15 @@
         <v>54.938049599999999</v>
       </c>
       <c r="D26">
-        <f>isotopes!D26</f>
-        <v>100</v>
+        <f>isotopes!D26/100</f>
+        <v>1</v>
       </c>
       <c r="E26">
         <f>IF(isotopes!E26-C26&lt;0,0,isotopes!E26-C26)</f>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>isotopes!F26</f>
+        <f>isotopes!F26/100</f>
         <v>0</v>
       </c>
       <c r="G26">
@@ -8762,7 +8977,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <f>isotopes!H26</f>
+        <f>isotopes!H26/100</f>
         <v>0</v>
       </c>
       <c r="I26">
@@ -8801,8 +9016,22 @@
         <f>isotopes!Q26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V26">
+        <v>198.13030075</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="1"/>
+        <v>3.0076006200000052</v>
+      </c>
+      <c r="X26">
+        <v>9.0274999999999994E-2</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="0"/>
+        <v>9.0274999999999991E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>isotopes!A27</f>
         <v>Fe</v>
@@ -8816,24 +9045,24 @@
         <v>53.939614800000001</v>
       </c>
       <c r="D27">
-        <f>isotopes!D27</f>
-        <v>5.8449999999999998</v>
+        <f>isotopes!D27/100</f>
+        <v>5.8449999999999995E-2</v>
       </c>
       <c r="E27">
         <f>IF(isotopes!E27-C27&lt;0,0,isotopes!E27-C27)</f>
         <v>1.9953272999999996</v>
       </c>
       <c r="F27">
-        <f>isotopes!F27</f>
-        <v>91.754000000000005</v>
+        <f>isotopes!F27/100</f>
+        <v>0.91754000000000002</v>
       </c>
       <c r="G27">
         <f>IF(isotopes!G27-C27&lt;0,0,isotopes!G27-C27)</f>
         <v>2.9957838999999993</v>
       </c>
       <c r="H27">
-        <f>isotopes!H27</f>
-        <v>2.1191</v>
+        <f>isotopes!H27/100</f>
+        <v>2.1191000000000002E-2</v>
       </c>
       <c r="I27">
         <f>isotopes!I27</f>
@@ -8872,7 +9101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>isotopes!A28</f>
         <v>Co</v>
@@ -8886,15 +9115,15 @@
         <v>58.933200200000002</v>
       </c>
       <c r="D28">
-        <f>isotopes!D28</f>
-        <v>100</v>
+        <f>isotopes!D28/100</f>
+        <v>1</v>
       </c>
       <c r="E28">
         <f>IF(isotopes!E28-C28&lt;0,0,isotopes!E28-C28)</f>
         <v>0</v>
       </c>
       <c r="F28">
-        <f>isotopes!F28</f>
+        <f>isotopes!F28/100</f>
         <v>0</v>
       </c>
       <c r="G28">
@@ -8902,7 +9131,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <f>isotopes!H28</f>
+        <f>isotopes!H28/100</f>
         <v>0</v>
       </c>
       <c r="I28">
@@ -8941,8 +9170,18 @@
         <f>isotopes!Q28</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V28">
+        <v>195.12270013</v>
+      </c>
+      <c r="X28">
+        <v>100</v>
+      </c>
+      <c r="Y28">
+        <f>X28/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>isotopes!A29</f>
         <v>Ni</v>
@@ -8956,24 +9195,24 @@
         <v>57.935347899999996</v>
       </c>
       <c r="D29">
-        <f>isotopes!D29</f>
-        <v>68.076899999999995</v>
+        <f>isotopes!D29/100</f>
+        <v>0.68076899999999996</v>
       </c>
       <c r="E29">
         <f>IF(isotopes!E29-C29&lt;0,0,isotopes!E29-C29)</f>
         <v>1.9954427000000052</v>
       </c>
       <c r="F29">
-        <f>isotopes!F29</f>
-        <v>26.223099999999999</v>
+        <f>isotopes!F29/100</f>
+        <v>0.26223099999999999</v>
       </c>
       <c r="G29">
         <f>IF(isotopes!G29-C29&lt;0,0,isotopes!G29-C29)</f>
         <v>2.9957125000000033</v>
       </c>
       <c r="H29">
-        <f>isotopes!H29</f>
-        <v>1.1398999999999999</v>
+        <f>isotopes!H29/100</f>
+        <v>1.1398999999999999E-2</v>
       </c>
       <c r="I29">
         <f>isotopes!I29</f>
@@ -9011,8 +9250,22 @@
         <f>isotopes!Q29</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V29">
+        <v>196.12605497000001</v>
+      </c>
+      <c r="W29">
+        <f>V29-$V$28</f>
+        <v>1.0033548400000143</v>
+      </c>
+      <c r="X29">
+        <v>8.6525829999999999</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Y36" si="2">X29/100</f>
+        <v>8.6525829999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>isotopes!A30</f>
         <v>Cu</v>
@@ -9026,23 +9279,23 @@
         <v>62.929601099999999</v>
       </c>
       <c r="D30">
-        <f>isotopes!D30</f>
-        <v>69.174000000000007</v>
+        <f>isotopes!D30/100</f>
+        <v>0.69174000000000002</v>
       </c>
       <c r="E30">
         <f>IF(isotopes!E30-C30&lt;0,0,isotopes!E30-C30)</f>
         <v>1.9981925999999959</v>
       </c>
       <c r="F30">
-        <f>isotopes!F30</f>
-        <v>30.826000000000001</v>
+        <f>isotopes!F30/100</f>
+        <v>0.30825999999999998</v>
       </c>
       <c r="G30">
         <f>IF(isotopes!G30-C30&lt;0,0,isotopes!G30-C30)</f>
         <v>0</v>
       </c>
       <c r="H30">
-        <f>isotopes!H30</f>
+        <f>isotopes!H30/100</f>
         <v>0</v>
       </c>
       <c r="I30">
@@ -9081,8 +9334,26 @@
         <f>isotopes!Q30</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V30">
+        <v>196.12691701</v>
+      </c>
+      <c r="W30">
+        <f t="shared" ref="W30:W36" si="3">V30-$V$28</f>
+        <v>1.0042168800000013</v>
+      </c>
+      <c r="X30">
+        <v>0.19046299999999999</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="2"/>
+        <v>1.90463E-3</v>
+      </c>
+      <c r="AA30">
+        <f>8*(8-1)*0.0058</f>
+        <v>0.32479999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>isotopes!A31</f>
         <v>Zn</v>
@@ -9096,24 +9367,24 @@
         <v>63.929146600000003</v>
       </c>
       <c r="D31">
-        <f>isotopes!D31</f>
-        <v>48.63</v>
+        <f>isotopes!D31/100</f>
+        <v>0.48630000000000001</v>
       </c>
       <c r="E31">
         <f>IF(isotopes!E31-C31&lt;0,0,isotopes!E31-C31)</f>
         <v>1.9968902000000028</v>
       </c>
       <c r="F31">
-        <f>isotopes!F31</f>
-        <v>27.9</v>
+        <f>isotopes!F31/100</f>
+        <v>0.27899999999999997</v>
       </c>
       <c r="G31">
         <f>IF(isotopes!G31-C31&lt;0,0,isotopes!G31-C31)</f>
         <v>2.9979842999999917</v>
       </c>
       <c r="H31">
-        <f>isotopes!H31</f>
-        <v>4.0999999999999996</v>
+        <f>isotopes!H31/100</f>
+        <v>4.0999999999999995E-2</v>
       </c>
       <c r="I31">
         <f>isotopes!I31</f>
@@ -9151,8 +9422,22 @@
         <f>isotopes!Q31</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V31">
+        <v>196.12897687</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="3"/>
+        <v>1.0062767400000041</v>
+      </c>
+      <c r="X31">
+        <v>0.218525</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="2"/>
+        <v>2.1852500000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>isotopes!A32</f>
         <v>Ga</v>
@@ -9166,23 +9451,23 @@
         <v>68.925580999999994</v>
       </c>
       <c r="D32">
-        <f>isotopes!D32</f>
-        <v>60.107900000000001</v>
+        <f>isotopes!D32/100</f>
+        <v>0.60107900000000003</v>
       </c>
       <c r="E32">
         <f>IF(isotopes!E32-C32&lt;0,0,isotopes!E32-C32)</f>
         <v>1.999124000000009</v>
       </c>
       <c r="F32">
-        <f>isotopes!F32</f>
-        <v>39.892099999999999</v>
+        <f>isotopes!F32/100</f>
+        <v>0.39892099999999997</v>
       </c>
       <c r="G32">
         <f>IF(isotopes!G32-C32&lt;0,0,isotopes!G32-C32)</f>
         <v>0</v>
       </c>
       <c r="H32">
-        <f>isotopes!H32</f>
+        <f>isotopes!H32/100</f>
         <v>0</v>
       </c>
       <c r="I32">
@@ -9221,8 +9506,22 @@
         <f>isotopes!Q32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V32">
+        <v>197.12694590999999</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="3"/>
+        <v>2.0042457799999909</v>
+      </c>
+      <c r="X32">
+        <v>1.0274970000000001</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="2"/>
+        <v>1.0274970000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>isotopes!A33</f>
         <v>Ge</v>
@@ -9236,24 +9535,24 @@
         <v>69.924250400000005</v>
       </c>
       <c r="D33">
-        <f>isotopes!D33</f>
-        <v>21.234000000000002</v>
+        <f>isotopes!D33/100</f>
+        <v>0.21234000000000003</v>
       </c>
       <c r="E33">
         <f>IF(isotopes!E33-C33&lt;0,0,isotopes!E33-C33)</f>
         <v>1.9978258000000011</v>
       </c>
       <c r="F33">
-        <f>isotopes!F33</f>
-        <v>27.661999999999999</v>
+        <f>isotopes!F33/100</f>
+        <v>0.27661999999999998</v>
       </c>
       <c r="G33">
         <f>IF(isotopes!G33-C33&lt;0,0,isotopes!G33-C33)</f>
         <v>2.9992089999999934</v>
       </c>
       <c r="H33">
-        <f>isotopes!H33</f>
-        <v>7.7169999999999996</v>
+        <f>isotopes!H33/100</f>
+        <v>7.7170000000000002E-2</v>
       </c>
       <c r="I33">
         <f>isotopes!I33</f>
@@ -9291,8 +9590,22 @@
         <f>isotopes!Q33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V33">
+        <v>197.12940981</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="3"/>
+        <v>2.0067096800000002</v>
+      </c>
+      <c r="X33">
+        <v>0.327544</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="2"/>
+        <v>3.2754400000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>isotopes!A34</f>
         <v>As</v>
@@ -9306,15 +9619,15 @@
         <v>74.921596399999999</v>
       </c>
       <c r="D34">
-        <f>isotopes!D34</f>
-        <v>100</v>
+        <f>isotopes!D34/100</f>
+        <v>1</v>
       </c>
       <c r="E34">
         <f>IF(isotopes!E34-C34&lt;0,0,isotopes!E34-C34)</f>
         <v>0</v>
       </c>
       <c r="F34">
-        <f>isotopes!F34</f>
+        <f>isotopes!F34/100</f>
         <v>0</v>
       </c>
       <c r="G34">
@@ -9322,7 +9635,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <f>isotopes!H34</f>
+        <f>isotopes!H34/100</f>
         <v>0</v>
       </c>
       <c r="I34">
@@ -9361,8 +9674,22 @@
         <f>isotopes!Q34</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V34">
+        <v>197.13027185000001</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="3"/>
+        <v>2.0075717200000156</v>
+      </c>
+      <c r="X34">
+        <v>1.6480000000000002E-2</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="2"/>
+        <v>1.6480000000000002E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>isotopes!A35</f>
         <v>Se</v>
@@ -9376,24 +9703,24 @@
         <v>73.922476599999996</v>
       </c>
       <c r="D35">
-        <f>isotopes!D35</f>
-        <v>0.88900000000000001</v>
+        <f>isotopes!D35/100</f>
+        <v>8.8900000000000003E-3</v>
       </c>
       <c r="E35">
         <f>IF(isotopes!E35-C35&lt;0,0,isotopes!E35-C35)</f>
         <v>1.9967375000000089</v>
       </c>
       <c r="F35">
-        <f>isotopes!F35</f>
-        <v>9.3659999999999997</v>
+        <f>isotopes!F35/100</f>
+        <v>9.3659999999999993E-2</v>
       </c>
       <c r="G35">
         <f>IF(isotopes!G35-C35&lt;0,0,isotopes!G35-C35)</f>
         <v>2.9974380000000025</v>
       </c>
       <c r="H35">
-        <f>isotopes!H35</f>
-        <v>7.6349999999999998</v>
+        <f>isotopes!H35/100</f>
+        <v>7.6350000000000001E-2</v>
       </c>
       <c r="I35">
         <f>isotopes!I35</f>
@@ -9431,8 +9758,22 @@
         <f>isotopes!Q35</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V35">
+        <v>197.13233170999999</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="3"/>
+        <v>2.00963157999999</v>
+      </c>
+      <c r="X35">
+        <v>1.8908000000000001E-2</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="2"/>
+        <v>1.8908E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>isotopes!A36</f>
         <v>Br</v>
@@ -9446,23 +9787,23 @@
         <v>78.918337600000001</v>
       </c>
       <c r="D36">
-        <f>isotopes!D36</f>
-        <v>50.686</v>
+        <f>isotopes!D36/100</f>
+        <v>0.50685999999999998</v>
       </c>
       <c r="E36">
         <f>IF(isotopes!E36-C36&lt;0,0,isotopes!E36-C36)</f>
         <v>1.9979534000000001</v>
       </c>
       <c r="F36">
-        <f>isotopes!F36</f>
-        <v>49.314</v>
+        <f>isotopes!F36/100</f>
+        <v>0.49314000000000002</v>
       </c>
       <c r="G36">
         <f>IF(isotopes!G36-C36&lt;0,0,isotopes!G36-C36)</f>
         <v>0</v>
       </c>
       <c r="H36">
-        <f>isotopes!H36</f>
+        <f>isotopes!H36/100</f>
         <v>0</v>
       </c>
       <c r="I36">
@@ -9501,8 +9842,22 @@
         <f>isotopes!Q36</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V36">
+        <v>198.13030075</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="3"/>
+        <v>3.0076006200000052</v>
+      </c>
+      <c r="X36">
+        <v>8.8904999999999998E-2</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="2"/>
+        <v>8.8904999999999995E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>isotopes!A37</f>
         <v>Kr</v>
@@ -9516,24 +9871,24 @@
         <v>77.920385999999993</v>
       </c>
       <c r="D37">
-        <f>isotopes!D37</f>
-        <v>0.35350999999999999</v>
+        <f>isotopes!D37/100</f>
+        <v>3.5350999999999998E-3</v>
       </c>
       <c r="E37">
         <f>IF(isotopes!E37-C37&lt;0,0,isotopes!E37-C37)</f>
         <v>1.9959920000000011</v>
       </c>
       <c r="F37">
-        <f>isotopes!F37</f>
-        <v>2.2808600000000001</v>
+        <f>isotopes!F37/100</f>
+        <v>2.2808600000000002E-2</v>
       </c>
       <c r="G37">
         <f>IF(isotopes!G37-C37&lt;0,0,isotopes!G37-C37)</f>
         <v>3.9930986000000104</v>
       </c>
       <c r="H37">
-        <f>isotopes!H37</f>
-        <v>11.58304</v>
+        <f>isotopes!H37/100</f>
+        <v>0.1158304</v>
       </c>
       <c r="I37">
         <f>isotopes!I37</f>
@@ -9572,7 +9927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>isotopes!A38</f>
         <v>Rb</v>
@@ -9586,23 +9941,23 @@
         <v>84.911789299999995</v>
       </c>
       <c r="D38">
-        <f>isotopes!D38</f>
-        <v>72.165400000000005</v>
+        <f>isotopes!D38/100</f>
+        <v>0.72165400000000002</v>
       </c>
       <c r="E38">
         <f>IF(isotopes!E38-C38&lt;0,0,isotopes!E38-C38)</f>
         <v>1.9973942000000022</v>
       </c>
       <c r="F38">
-        <f>isotopes!F38</f>
-        <v>27.834599999999998</v>
+        <f>isotopes!F38/100</f>
+        <v>0.27834599999999998</v>
       </c>
       <c r="G38">
         <f>IF(isotopes!G38-C38&lt;0,0,isotopes!G38-C38)</f>
         <v>0</v>
       </c>
       <c r="H38">
-        <f>isotopes!H38</f>
+        <f>isotopes!H38/100</f>
         <v>0</v>
       </c>
       <c r="I38">
@@ -9642,7 +9997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>isotopes!A39</f>
         <v>Sr</v>
@@ -9656,24 +10011,24 @@
         <v>83.913425000000004</v>
       </c>
       <c r="D39">
-        <f>isotopes!D39</f>
-        <v>0.55740000000000001</v>
+        <f>isotopes!D39/100</f>
+        <v>5.574E-3</v>
       </c>
       <c r="E39">
         <f>IF(isotopes!E39-C39&lt;0,0,isotopes!E39-C39)</f>
         <v>1.9958373999999992</v>
       </c>
       <c r="F39">
-        <f>isotopes!F39</f>
-        <v>9.8566000000000003</v>
+        <f>isotopes!F39/100</f>
+        <v>9.8566000000000001E-2</v>
       </c>
       <c r="G39">
         <f>IF(isotopes!G39-C39&lt;0,0,isotopes!G39-C39)</f>
         <v>2.9954542999999916</v>
       </c>
       <c r="H39">
-        <f>isotopes!H39</f>
-        <v>7.0015000000000001</v>
+        <f>isotopes!H39/100</f>
+        <v>7.0014999999999994E-2</v>
       </c>
       <c r="I39">
         <f>isotopes!I39</f>
@@ -9711,8 +10066,18 @@
         <f>isotopes!Q39</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V39">
+        <v>388.10586024999998</v>
+      </c>
+      <c r="X39">
+        <v>100</v>
+      </c>
+      <c r="Y39">
+        <f>X39/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>isotopes!A40</f>
         <v>Y</v>
@@ -9726,15 +10091,15 @@
         <v>88.905847899999998</v>
       </c>
       <c r="D40">
-        <f>isotopes!D40</f>
-        <v>100</v>
+        <f>isotopes!D40/100</f>
+        <v>1</v>
       </c>
       <c r="E40">
         <f>IF(isotopes!E40-C40&lt;0,0,isotopes!E40-C40)</f>
         <v>0</v>
       </c>
       <c r="F40">
-        <f>isotopes!F40</f>
+        <f>isotopes!F40/100</f>
         <v>0</v>
       </c>
       <c r="G40">
@@ -9742,7 +10107,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <f>isotopes!H40</f>
+        <f>isotopes!H40/100</f>
         <v>0</v>
       </c>
       <c r="I40">
@@ -9781,8 +10146,22 @@
         <f>isotopes!Q40</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V40">
+        <v>389.10281061000001</v>
+      </c>
+      <c r="W40">
+        <f>V40-$V$39</f>
+        <v>0.99695036000002801</v>
+      </c>
+      <c r="X40">
+        <v>1.053474</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" ref="Y40:Y49" si="4">X40/100</f>
+        <v>1.0534740000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>isotopes!A41</f>
         <v>Zr</v>
@@ -9796,24 +10175,24 @@
         <v>89.904703699999999</v>
       </c>
       <c r="D41">
-        <f>isotopes!D41</f>
-        <v>51.451999999999998</v>
+        <f>isotopes!D41/100</f>
+        <v>0.51451999999999998</v>
       </c>
       <c r="E41">
         <f>IF(isotopes!E41-C41&lt;0,0,isotopes!E41-C41)</f>
         <v>1.000941300000008</v>
       </c>
       <c r="F41">
-        <f>isotopes!F41</f>
-        <v>11.223000000000001</v>
+        <f>isotopes!F41/100</f>
+        <v>0.11223000000000001</v>
       </c>
       <c r="G41">
         <f>IF(isotopes!G41-C41&lt;0,0,isotopes!G41-C41)</f>
         <v>2.0003363999999948</v>
       </c>
       <c r="H41">
-        <f>isotopes!H41</f>
-        <v>17.146000000000001</v>
+        <f>isotopes!H41/100</f>
+        <v>0.17146</v>
       </c>
       <c r="I41">
         <f>isotopes!I41</f>
@@ -9851,8 +10230,22 @@
         <f>isotopes!Q41</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V41">
+        <v>389.10925011</v>
+      </c>
+      <c r="W41">
+        <f t="shared" ref="W41:W50" si="5">V41-$V$39</f>
+        <v>1.0033898600000271</v>
+      </c>
+      <c r="X41">
+        <v>21.020198000000001</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="4"/>
+        <v>0.21020198000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>isotopes!A42</f>
         <v>Nb</v>
@@ -9866,15 +10259,15 @@
         <v>92.906377500000005</v>
       </c>
       <c r="D42">
-        <f>isotopes!D42</f>
-        <v>100</v>
+        <f>isotopes!D42/100</f>
+        <v>1</v>
       </c>
       <c r="E42">
         <f>IF(isotopes!E42-C42&lt;0,0,isotopes!E42-C42)</f>
         <v>0</v>
       </c>
       <c r="F42">
-        <f>isotopes!F42</f>
+        <f>isotopes!F42/100</f>
         <v>0</v>
       </c>
       <c r="G42">
@@ -9882,7 +10275,7 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <f>isotopes!H42</f>
+        <f>isotopes!H42/100</f>
         <v>0</v>
       </c>
       <c r="I42">
@@ -9921,8 +10314,22 @@
         <f>isotopes!Q42</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V42">
+        <v>390.10293614</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="5"/>
+        <v>1.9970758900000192</v>
+      </c>
+      <c r="X42">
+        <v>32.395021999999997</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="4"/>
+        <v>0.32395021999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>isotopes!A43</f>
         <v>Mo</v>
@@ -9936,24 +10343,24 @@
         <v>91.906809999999993</v>
       </c>
       <c r="D43">
-        <f>isotopes!D43</f>
-        <v>14.8362</v>
+        <f>isotopes!D43/100</f>
+        <v>0.14836199999999999</v>
       </c>
       <c r="E43">
         <f>IF(isotopes!E43-C43&lt;0,0,isotopes!E43-C43)</f>
         <v>1.9982776000000086</v>
       </c>
       <c r="F43">
-        <f>isotopes!F43</f>
-        <v>9.2466000000000008</v>
+        <f>isotopes!F43/100</f>
+        <v>9.2466000000000007E-2</v>
       </c>
       <c r="G43">
         <f>IF(isotopes!G43-C43&lt;0,0,isotopes!G43-C43)</f>
         <v>2.999031500000001</v>
       </c>
       <c r="H43">
-        <f>isotopes!H43</f>
-        <v>15.9201</v>
+        <f>isotopes!H43/100</f>
+        <v>0.15920100000000001</v>
       </c>
       <c r="I43">
         <f>isotopes!I43</f>
@@ -9991,8 +10398,22 @@
         <f>isotopes!Q43</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V43">
+        <v>390.11197895999999</v>
+      </c>
+      <c r="W43">
+        <f>V43-$V$39</f>
+        <v>2.0061187100000097</v>
+      </c>
+      <c r="X43">
+        <v>2.9053339999999999</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="4"/>
+        <v>2.9053339999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>isotopes!A44</f>
         <v>Ru</v>
@@ -10006,24 +10427,24 @@
         <v>95.907597999999993</v>
       </c>
       <c r="D44">
-        <f>isotopes!D44</f>
-        <v>5.5419999999999998</v>
+        <f>isotopes!D44/100</f>
+        <v>5.5419999999999997E-2</v>
       </c>
       <c r="E44">
         <f>IF(isotopes!E44-C44&lt;0,0,isotopes!E44-C44)</f>
         <v>1.9976890000000083</v>
       </c>
       <c r="F44">
-        <f>isotopes!F44</f>
-        <v>1.8688</v>
+        <f>isotopes!F44/100</f>
+        <v>1.8688E-2</v>
       </c>
       <c r="G44">
         <f>IF(isotopes!G44-C44&lt;0,0,isotopes!G44-C44)</f>
         <v>2.998341300000007</v>
       </c>
       <c r="H44">
-        <f>isotopes!H44</f>
-        <v>12.757899999999999</v>
+        <f>isotopes!H44/100</f>
+        <v>0.127579</v>
       </c>
       <c r="I44">
         <f>isotopes!I44</f>
@@ -10061,8 +10482,22 @@
         <f>isotopes!Q44</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V44">
+        <v>391.09979827000001</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="5"/>
+        <v>2.9939380200000301</v>
+      </c>
+      <c r="X44">
+        <v>0.329515</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="4"/>
+        <v>3.2951500000000002E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>isotopes!A45</f>
         <v>Rh</v>
@@ -10076,15 +10511,15 @@
         <v>102.90550399999999</v>
       </c>
       <c r="D45">
-        <f>isotopes!D45</f>
-        <v>100</v>
+        <f>isotopes!D45/100</f>
+        <v>1</v>
       </c>
       <c r="E45">
         <f>IF(isotopes!E45-C45&lt;0,0,isotopes!E45-C45)</f>
         <v>0</v>
       </c>
       <c r="F45">
-        <f>isotopes!F45</f>
+        <f>isotopes!F45/100</f>
         <v>0</v>
       </c>
       <c r="G45">
@@ -10092,7 +10527,7 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <f>isotopes!H45</f>
+        <f>isotopes!H45/100</f>
         <v>0</v>
       </c>
       <c r="I45">
@@ -10131,8 +10566,22 @@
         <f>isotopes!Q45</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V45">
+        <v>391.10630902999998</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="5"/>
+        <v>3.0004487799999993</v>
+      </c>
+      <c r="X45">
+        <v>6.794295</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="4"/>
+        <v>6.7942950000000002E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>isotopes!A46</f>
         <v>Pd</v>
@@ -10146,24 +10595,24 @@
         <v>101.905608</v>
       </c>
       <c r="D46">
-        <f>isotopes!D46</f>
-        <v>1.02</v>
+        <f>isotopes!D46/100</f>
+        <v>1.0200000000000001E-2</v>
       </c>
       <c r="E46">
         <f>IF(isotopes!E46-C46&lt;0,0,isotopes!E46-C46)</f>
         <v>1.9984269999999924</v>
       </c>
       <c r="F46">
-        <f>isotopes!F46</f>
-        <v>11.14</v>
+        <f>isotopes!F46/100</f>
+        <v>0.1114</v>
       </c>
       <c r="G46">
         <f>IF(isotopes!G46-C46&lt;0,0,isotopes!G46-C46)</f>
         <v>2.9994760000000014</v>
       </c>
       <c r="H46">
-        <f>isotopes!H46</f>
-        <v>22.33</v>
+        <f>isotopes!H46/100</f>
+        <v>0.22329999999999997</v>
       </c>
       <c r="I46">
         <f>isotopes!I46</f>
@@ -10201,8 +10650,22 @@
         <f>isotopes!Q46</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V46">
+        <v>391.11461315000003</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="5"/>
+        <v>3.0087529000000472</v>
+      </c>
+      <c r="X46">
+        <v>0.29095300000000002</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="4"/>
+        <v>2.90953E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>isotopes!A47</f>
         <v>Ag</v>
@@ -10216,23 +10679,23 @@
         <v>106.90509299999999</v>
       </c>
       <c r="D47">
-        <f>isotopes!D47</f>
-        <v>51.839199999999998</v>
+        <f>isotopes!D47/100</f>
+        <v>0.51839199999999996</v>
       </c>
       <c r="E47">
         <f>IF(isotopes!E47-C47&lt;0,0,isotopes!E47-C47)</f>
         <v>1.9996630000000124</v>
       </c>
       <c r="F47">
-        <f>isotopes!F47</f>
-        <v>48.160800000000002</v>
+        <f>isotopes!F47/100</f>
+        <v>0.48160800000000004</v>
       </c>
       <c r="G47">
         <f>IF(isotopes!G47-C47&lt;0,0,isotopes!G47-C47)</f>
         <v>0</v>
       </c>
       <c r="H47">
-        <f>isotopes!H47</f>
+        <f>isotopes!H47/100</f>
         <v>0</v>
       </c>
       <c r="I47">
@@ -10271,8 +10734,22 @@
         <f>isotopes!Q47</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V47">
+        <v>392.10857075000001</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="5"/>
+        <v>4.0027105000000347</v>
+      </c>
+      <c r="X47">
+        <v>1.010194</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="4"/>
+        <v>1.010194E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>isotopes!A48</f>
         <v>Cd</v>
@@ -10286,24 +10763,24 @@
         <v>105.906458</v>
       </c>
       <c r="D48">
-        <f>isotopes!D48</f>
-        <v>1.25</v>
+        <f>isotopes!D48/100</f>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E48">
         <f>IF(isotopes!E48-C48&lt;0,0,isotopes!E48-C48)</f>
         <v>1.9977250000000026</v>
       </c>
       <c r="F48">
-        <f>isotopes!F48</f>
-        <v>0.89</v>
+        <f>isotopes!F48/100</f>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="G48">
         <f>IF(isotopes!G48-C48&lt;0,0,isotopes!G48-C48)</f>
         <v>3.9965480000000042</v>
       </c>
       <c r="H48">
-        <f>isotopes!H48</f>
-        <v>12.49</v>
+        <f>isotopes!H48/100</f>
+        <v>0.1249</v>
       </c>
       <c r="I48">
         <f>isotopes!I48</f>
@@ -10341,8 +10818,22 @@
         <f>isotopes!Q48</f>
         <v>115.90475499999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V48">
+        <v>392.11700474000003</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="5"/>
+        <v>4.0111444900000492</v>
+      </c>
+      <c r="X48">
+        <v>1.6211E-2</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="4"/>
+        <v>1.6211E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>isotopes!A49</f>
         <v>In</v>
@@ -10356,23 +10847,23 @@
         <v>112.904061</v>
       </c>
       <c r="D49">
-        <f>isotopes!D49</f>
-        <v>4.2880000000000003</v>
+        <f>isotopes!D49/100</f>
+        <v>4.2880000000000001E-2</v>
       </c>
       <c r="E49">
         <f>IF(isotopes!E49-C49&lt;0,0,isotopes!E49-C49)</f>
         <v>1.9998170000000073</v>
       </c>
       <c r="F49">
-        <f>isotopes!F49</f>
-        <v>95.712000000000003</v>
+        <f>isotopes!F49/100</f>
+        <v>0.95712000000000008</v>
       </c>
       <c r="G49">
         <f>IF(isotopes!G49-C49&lt;0,0,isotopes!G49-C49)</f>
         <v>0</v>
       </c>
       <c r="H49">
-        <f>isotopes!H49</f>
+        <f>isotopes!H49/100</f>
         <v>0</v>
       </c>
       <c r="I49">
@@ -10411,8 +10902,22 @@
         <f>isotopes!Q49</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V49">
+        <v>393.11154697000001</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="5"/>
+        <v>5.0056867200000283</v>
+      </c>
+      <c r="X49">
+        <v>9.4477000000000005E-2</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="4"/>
+        <v>9.4477000000000005E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>isotopes!A50</f>
         <v>Sn</v>
@@ -10426,24 +10931,24 @@
         <v>111.904821</v>
       </c>
       <c r="D50">
-        <f>isotopes!D50</f>
-        <v>0.97299999999999998</v>
+        <f>isotopes!D50/100</f>
+        <v>9.7299999999999991E-3</v>
       </c>
       <c r="E50">
         <f>IF(isotopes!E50-C50&lt;0,0,isotopes!E50-C50)</f>
         <v>1.9979610000000037</v>
       </c>
       <c r="F50">
-        <f>isotopes!F50</f>
-        <v>0.65900000000000003</v>
+        <f>isotopes!F50/100</f>
+        <v>6.5900000000000004E-3</v>
       </c>
       <c r="G50">
         <f>IF(isotopes!G50-C50&lt;0,0,isotopes!G50-C50)</f>
         <v>2.9985250000000008</v>
       </c>
       <c r="H50">
-        <f>isotopes!H50</f>
-        <v>0.33900000000000002</v>
+        <f>isotopes!H50/100</f>
+        <v>3.3900000000000002E-3</v>
       </c>
       <c r="I50">
         <f>isotopes!I50</f>
@@ -10482,7 +10987,7 @@
         <v>119.9021966</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>isotopes!A51</f>
         <v>Sb</v>
@@ -10496,23 +11001,23 @@
         <v>120.903818</v>
       </c>
       <c r="D51">
-        <f>isotopes!D51</f>
-        <v>57.213000000000001</v>
+        <f>isotopes!D51/100</f>
+        <v>0.57213000000000003</v>
       </c>
       <c r="E51">
         <f>IF(isotopes!E51-C51&lt;0,0,isotopes!E51-C51)</f>
         <v>2.0003976999999935</v>
       </c>
       <c r="F51">
-        <f>isotopes!F51</f>
-        <v>42.786999999999999</v>
+        <f>isotopes!F51/100</f>
+        <v>0.42786999999999997</v>
       </c>
       <c r="G51">
         <f>IF(isotopes!G51-C51&lt;0,0,isotopes!G51-C51)</f>
         <v>0</v>
       </c>
       <c r="H51">
-        <f>isotopes!H51</f>
+        <f>isotopes!H51/100</f>
         <v>0</v>
       </c>
       <c r="I51">
@@ -10552,7 +11057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>isotopes!A52</f>
         <v>Te</v>
@@ -10566,24 +11071,24 @@
         <v>119.90402</v>
       </c>
       <c r="D52">
-        <f>isotopes!D52</f>
-        <v>9.6000000000000002E-2</v>
+        <f>isotopes!D52/100</f>
+        <v>9.6000000000000002E-4</v>
       </c>
       <c r="E52">
         <f>IF(isotopes!E52-C52&lt;0,0,isotopes!E52-C52)</f>
         <v>1.9990270999999922</v>
       </c>
       <c r="F52">
-        <f>isotopes!F52</f>
-        <v>2.6030000000000002</v>
+        <f>isotopes!F52/100</f>
+        <v>2.6030000000000001E-2</v>
       </c>
       <c r="G52">
         <f>IF(isotopes!G52-C52&lt;0,0,isotopes!G52-C52)</f>
         <v>3.0002530000000007</v>
       </c>
       <c r="H52">
-        <f>isotopes!H52</f>
-        <v>0.90800000000000003</v>
+        <f>isotopes!H52/100</f>
+        <v>9.0799999999999995E-3</v>
       </c>
       <c r="I52">
         <f>isotopes!I52</f>
@@ -10621,8 +11126,18 @@
         <f>isotopes!Q52</f>
         <v>129.90622279999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V52">
+        <v>388.10586024999998</v>
+      </c>
+      <c r="X52">
+        <v>100</v>
+      </c>
+      <c r="Y52">
+        <f>X52/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>isotopes!A53</f>
         <v>I</v>
@@ -10636,15 +11151,15 @@
         <v>126.90446799999999</v>
       </c>
       <c r="D53">
-        <f>isotopes!D53</f>
-        <v>100</v>
+        <f>isotopes!D53/100</f>
+        <v>1</v>
       </c>
       <c r="E53">
         <f>IF(isotopes!E53-C53&lt;0,0,isotopes!E53-C53)</f>
         <v>0</v>
       </c>
       <c r="F53">
-        <f>isotopes!F53</f>
+        <f>isotopes!F53/100</f>
         <v>0</v>
       </c>
       <c r="G53">
@@ -10652,7 +11167,7 @@
         <v>0</v>
       </c>
       <c r="H53">
-        <f>isotopes!H53</f>
+        <f>isotopes!H53/100</f>
         <v>0</v>
       </c>
       <c r="I53">
@@ -10691,8 +11206,22 @@
         <f>isotopes!Q53</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V53">
+        <v>389.10289520999999</v>
+      </c>
+      <c r="W53">
+        <f>V53-$V$52</f>
+        <v>0.99703496000000769</v>
+      </c>
+      <c r="X53">
+        <v>1.0959890000000001</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" ref="Y53:Y77" si="6">X53/100</f>
+        <v>1.0959890000000002E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>isotopes!A54</f>
         <v>Xe</v>
@@ -10706,24 +11235,24 @@
         <v>123.9058958</v>
       </c>
       <c r="D54">
-        <f>isotopes!D54</f>
-        <v>8.9130000000000001E-2</v>
+        <f>isotopes!D54/100</f>
+        <v>8.9130000000000003E-4</v>
       </c>
       <c r="E54">
         <f>IF(isotopes!E54-C54&lt;0,0,isotopes!E54-C54)</f>
         <v>1.9983732000000032</v>
       </c>
       <c r="F54">
-        <f>isotopes!F54</f>
-        <v>8.8800000000000004E-2</v>
+        <f>isotopes!F54/100</f>
+        <v>8.8800000000000001E-4</v>
       </c>
       <c r="G54">
         <f>IF(isotopes!G54-C54&lt;0,0,isotopes!G54-C54)</f>
         <v>3.9976345999999978</v>
       </c>
       <c r="H54">
-        <f>isotopes!H54</f>
-        <v>1.9173199999999999</v>
+        <f>isotopes!H54/100</f>
+        <v>1.9173199999999998E-2</v>
       </c>
       <c r="I54">
         <f>isotopes!I54</f>
@@ -10761,8 +11290,22 @@
         <f>isotopes!Q54</f>
         <v>133.9053945</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V54">
+        <v>389.10921509000002</v>
+      </c>
+      <c r="W54">
+        <f t="shared" ref="W54:W77" si="7">V54-$V$52</f>
+        <v>1.0033548400000427</v>
+      </c>
+      <c r="X54">
+        <v>20.549883999999999</v>
+      </c>
+      <c r="Y54">
+        <f t="shared" si="6"/>
+        <v>0.20549883999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>isotopes!A55</f>
         <v>Cs</v>
@@ -10776,15 +11319,15 @@
         <v>132.90544700000001</v>
       </c>
       <c r="D55">
-        <f>isotopes!D55</f>
-        <v>100</v>
+        <f>isotopes!D55/100</f>
+        <v>1</v>
       </c>
       <c r="E55">
         <f>IF(isotopes!E55-C55&lt;0,0,isotopes!E55-C55)</f>
         <v>0</v>
       </c>
       <c r="F55">
-        <f>isotopes!F55</f>
+        <f>isotopes!F55/100</f>
         <v>0</v>
       </c>
       <c r="G55">
@@ -10792,7 +11335,7 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <f>isotopes!H55</f>
+        <f>isotopes!H55/100</f>
         <v>0</v>
       </c>
       <c r="I55">
@@ -10831,8 +11374,22 @@
         <f>isotopes!Q55</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V55">
+        <v>389.11007712999998</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="7"/>
+        <v>1.0042168800000013</v>
+      </c>
+      <c r="X55">
+        <v>0.15237000000000001</v>
+      </c>
+      <c r="Y55">
+        <f t="shared" si="6"/>
+        <v>1.5237E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>isotopes!A56</f>
         <v>Ba</v>
@@ -10846,24 +11403,24 @@
         <v>129.90630999999999</v>
       </c>
       <c r="D56">
-        <f>isotopes!D56</f>
-        <v>0.10580000000000001</v>
+        <f>isotopes!D56/100</f>
+        <v>1.0580000000000001E-3</v>
       </c>
       <c r="E56">
         <f>IF(isotopes!E56-C56&lt;0,0,isotopes!E56-C56)</f>
         <v>1.9987460000000112</v>
       </c>
       <c r="F56">
-        <f>isotopes!F56</f>
-        <v>0.1012</v>
+        <f>isotopes!F56/100</f>
+        <v>1.0119999999999999E-3</v>
       </c>
       <c r="G56">
         <f>IF(isotopes!G56-C56&lt;0,0,isotopes!G56-C56)</f>
         <v>3.9981930000000148</v>
       </c>
       <c r="H56">
-        <f>isotopes!H56</f>
-        <v>2.4169999999999998</v>
+        <f>isotopes!H56/100</f>
+        <v>2.4169999999999997E-2</v>
       </c>
       <c r="I56">
         <f>isotopes!I56</f>
@@ -10901,8 +11458,22 @@
         <f>isotopes!Q56</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V56">
+        <v>389.11213699000001</v>
+      </c>
+      <c r="W56">
+        <f t="shared" si="7"/>
+        <v>1.0062767400000325</v>
+      </c>
+      <c r="X56">
+        <v>0.218525</v>
+      </c>
+      <c r="Y56">
+        <f t="shared" si="6"/>
+        <v>2.1852500000000001E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>isotopes!A57</f>
         <v>La</v>
@@ -10916,23 +11487,23 @@
         <v>137.907107</v>
       </c>
       <c r="D57">
-        <f>isotopes!D57</f>
-        <v>9.017E-2</v>
+        <f>isotopes!D57/100</f>
+        <v>9.0169999999999996E-4</v>
       </c>
       <c r="E57">
         <f>IF(isotopes!E57-C57&lt;0,0,isotopes!E57-C57)</f>
         <v>0.99924100000001204</v>
       </c>
       <c r="F57">
-        <f>isotopes!F57</f>
-        <v>99.909829999999999</v>
+        <f>isotopes!F57/100</f>
+        <v>0.99909829999999999</v>
       </c>
       <c r="G57">
         <f>IF(isotopes!G57-C57&lt;0,0,isotopes!G57-C57)</f>
         <v>0</v>
       </c>
       <c r="H57">
-        <f>isotopes!H57</f>
+        <f>isotopes!H57/100</f>
         <v>0</v>
       </c>
       <c r="I57">
@@ -10971,8 +11542,22 @@
         <f>isotopes!Q57</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V57">
+        <v>390.10291014000001</v>
+      </c>
+      <c r="W57">
+        <f t="shared" si="7"/>
+        <v>1.997049890000028</v>
+      </c>
+      <c r="X57">
+        <v>31.995775999999999</v>
+      </c>
+      <c r="Y57">
+        <f t="shared" si="6"/>
+        <v>0.31995775999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>isotopes!A58</f>
         <v>Ce</v>
@@ -10986,24 +11571,24 @@
         <v>135.90714</v>
       </c>
       <c r="D58">
-        <f>isotopes!D58</f>
-        <v>0.186</v>
+        <f>isotopes!D58/100</f>
+        <v>1.8599999999999999E-3</v>
       </c>
       <c r="E58">
         <f>IF(isotopes!E58-C58&lt;0,0,isotopes!E58-C58)</f>
         <v>1.9988460000000146</v>
       </c>
       <c r="F58">
-        <f>isotopes!F58</f>
-        <v>0.251</v>
+        <f>isotopes!F58/100</f>
+        <v>2.5100000000000001E-3</v>
       </c>
       <c r="G58">
         <f>IF(isotopes!G58-C58&lt;0,0,isotopes!G58-C58)</f>
         <v>3.9982940000000156</v>
       </c>
       <c r="H58">
-        <f>isotopes!H58</f>
-        <v>88.448999999999998</v>
+        <f>isotopes!H58/100</f>
+        <v>0.88449</v>
       </c>
       <c r="I58">
         <f>isotopes!I58</f>
@@ -11041,8 +11626,22 @@
         <f>isotopes!Q58</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V58">
+        <v>390.10625005000003</v>
+      </c>
+      <c r="W58">
+        <f t="shared" si="7"/>
+        <v>2.0003898000000504</v>
+      </c>
+      <c r="X58">
+        <v>0.22522500000000001</v>
+      </c>
+      <c r="Y58">
+        <f t="shared" si="6"/>
+        <v>2.2522499999999999E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>isotopes!A59</f>
         <v>Pr</v>
@@ -11056,15 +11655,15 @@
         <v>140.90764799999999</v>
       </c>
       <c r="D59">
-        <f>isotopes!D59</f>
-        <v>100</v>
+        <f>isotopes!D59/100</f>
+        <v>1</v>
       </c>
       <c r="E59">
         <f>IF(isotopes!E59-C59&lt;0,0,isotopes!E59-C59)</f>
         <v>0</v>
       </c>
       <c r="F59">
-        <f>isotopes!F59</f>
+        <f>isotopes!F59/100</f>
         <v>0</v>
       </c>
       <c r="G59">
@@ -11072,7 +11671,7 @@
         <v>0</v>
       </c>
       <c r="H59">
-        <f>isotopes!H59</f>
+        <f>isotopes!H59/100</f>
         <v>0</v>
       </c>
       <c r="I59">
@@ -11111,8 +11710,22 @@
         <f>isotopes!Q59</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V59">
+        <v>390.11010603</v>
+      </c>
+      <c r="W59">
+        <f t="shared" si="7"/>
+        <v>2.0042457800000193</v>
+      </c>
+      <c r="X59">
+        <v>0.82199699999999998</v>
+      </c>
+      <c r="Y59">
+        <f t="shared" si="6"/>
+        <v>8.2199700000000001E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>isotopes!A60</f>
         <v>Nd</v>
@@ -11126,24 +11739,24 @@
         <v>141.90771899999999</v>
       </c>
       <c r="D60">
-        <f>isotopes!D60</f>
-        <v>27.16</v>
+        <f>isotopes!D60/100</f>
+        <v>0.27160000000000001</v>
       </c>
       <c r="E60">
         <f>IF(isotopes!E60-C60&lt;0,0,isotopes!E60-C60)</f>
         <v>1.0020910000000072</v>
       </c>
       <c r="F60">
-        <f>isotopes!F60</f>
-        <v>12.18</v>
+        <f>isotopes!F60/100</f>
+        <v>0.12179999999999999</v>
       </c>
       <c r="G60">
         <f>IF(isotopes!G60-C60&lt;0,0,isotopes!G60-C60)</f>
         <v>2.002364</v>
       </c>
       <c r="H60">
-        <f>isotopes!H60</f>
-        <v>23.83</v>
+        <f>isotopes!H60/100</f>
+        <v>0.23829999999999998</v>
       </c>
       <c r="I60">
         <f>isotopes!I60</f>
@@ -11181,8 +11794,26 @@
         <f>isotopes!Q60</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V60">
+        <v>390.11256993000001</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="7"/>
+        <v>2.0067096800000286</v>
+      </c>
+      <c r="X60">
+        <v>2.0003579999999999</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="6"/>
+        <v>2.000358E-2</v>
+      </c>
+      <c r="AA60">
+        <f>((F7*F7)/2)*19*(19-1)</f>
+        <v>2.0985476363999996E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>isotopes!A61</f>
         <v>Sm</v>
@@ -11196,24 +11827,24 @@
         <v>143.91199499999999</v>
       </c>
       <c r="D61">
-        <f>isotopes!D61</f>
-        <v>3.0733999999999999</v>
+        <f>isotopes!D61/100</f>
+        <v>3.0733999999999997E-2</v>
       </c>
       <c r="E61">
         <f>IF(isotopes!E61-C61&lt;0,0,isotopes!E61-C61)</f>
         <v>3.0028980000000161</v>
       </c>
       <c r="F61">
-        <f>isotopes!F61</f>
-        <v>14.993399999999999</v>
+        <f>isotopes!F61/100</f>
+        <v>0.14993399999999998</v>
       </c>
       <c r="G61">
         <f>IF(isotopes!G61-C61&lt;0,0,isotopes!G61-C61)</f>
         <v>4.0028230000000065</v>
       </c>
       <c r="H61">
-        <f>isotopes!H61</f>
-        <v>11.240600000000001</v>
+        <f>isotopes!H61/100</f>
+        <v>0.11240600000000001</v>
       </c>
       <c r="I61">
         <f>isotopes!I61</f>
@@ -11251,8 +11882,22 @@
         <f>isotopes!Q61</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V61">
+        <v>390.11343197000002</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="7"/>
+        <v>2.007571720000044</v>
+      </c>
+      <c r="X61">
+        <v>3.1312E-2</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="6"/>
+        <v>3.1312000000000001E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>isotopes!A62</f>
         <v>Eu</v>
@@ -11266,23 +11911,23 @@
         <v>150.91984600000001</v>
       </c>
       <c r="D62">
-        <f>isotopes!D62</f>
-        <v>47.81</v>
+        <f>isotopes!D62/100</f>
+        <v>0.47810000000000002</v>
       </c>
       <c r="E62">
         <f>IF(isotopes!E62-C62&lt;0,0,isotopes!E62-C62)</f>
         <v>2.0013799999999833</v>
       </c>
       <c r="F62">
-        <f>isotopes!F62</f>
-        <v>52.19</v>
+        <f>isotopes!F62/100</f>
+        <v>0.52190000000000003</v>
       </c>
       <c r="G62">
         <f>IF(isotopes!G62-C62&lt;0,0,isotopes!G62-C62)</f>
         <v>0</v>
       </c>
       <c r="H62">
-        <f>isotopes!H62</f>
+        <f>isotopes!H62/100</f>
         <v>0</v>
       </c>
       <c r="I62">
@@ -11321,8 +11966,22 @@
         <f>isotopes!Q62</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V62">
+        <v>390.11549183</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="7"/>
+        <v>2.0096315800000184</v>
+      </c>
+      <c r="X62">
+        <v>4.4907000000000002E-2</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="6"/>
+        <v>4.4907000000000004E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>isotopes!A63</f>
         <v>Gd</v>
@@ -11336,24 +11995,24 @@
         <v>151.91978800000001</v>
       </c>
       <c r="D63">
-        <f>isotopes!D63</f>
-        <v>0.2029</v>
+        <f>isotopes!D63/100</f>
+        <v>2.029E-3</v>
       </c>
       <c r="E63">
         <f>IF(isotopes!E63-C63&lt;0,0,isotopes!E63-C63)</f>
         <v>2.0010739999999885</v>
       </c>
       <c r="F63">
-        <f>isotopes!F63</f>
-        <v>2.1808999999999998</v>
+        <f>isotopes!F63/100</f>
+        <v>2.1808999999999999E-2</v>
       </c>
       <c r="G63">
         <f>IF(isotopes!G63-C63&lt;0,0,isotopes!G63-C63)</f>
         <v>3.0028309999999863</v>
       </c>
       <c r="H63">
-        <f>isotopes!H63</f>
-        <v>14.799799999999999</v>
+        <f>isotopes!H63/100</f>
+        <v>0.14799799999999999</v>
       </c>
       <c r="I63">
         <f>isotopes!I63</f>
@@ -11391,8 +12050,22 @@
         <f>isotopes!Q63</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V63">
+        <v>391.09994510000001</v>
+      </c>
+      <c r="W63">
+        <f t="shared" si="7"/>
+        <v>2.9940848500000357</v>
+      </c>
+      <c r="X63">
+        <v>0.35066999999999998</v>
+      </c>
+      <c r="Y63">
+        <f t="shared" si="6"/>
+        <v>3.5066999999999997E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>isotopes!A64</f>
         <v>Tb</v>
@@ -11406,15 +12079,15 @@
         <v>158.925343</v>
       </c>
       <c r="D64">
-        <f>isotopes!D64</f>
-        <v>100</v>
+        <f>isotopes!D64/100</f>
+        <v>1</v>
       </c>
       <c r="E64">
         <f>IF(isotopes!E64-C64&lt;0,0,isotopes!E64-C64)</f>
         <v>0</v>
       </c>
       <c r="F64">
-        <f>isotopes!F64</f>
+        <f>isotopes!F64/100</f>
         <v>0</v>
       </c>
       <c r="G64">
@@ -11422,7 +12095,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <f>isotopes!H64</f>
+        <f>isotopes!H64/100</f>
         <v>0</v>
       </c>
       <c r="I64">
@@ -11461,8 +12134,22 @@
         <f>isotopes!Q64</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V64">
+        <v>391.10626497999999</v>
+      </c>
+      <c r="W64">
+        <f t="shared" si="7"/>
+        <v>3.0004047300000138</v>
+      </c>
+      <c r="X64">
+        <v>6.5750950000000001</v>
+      </c>
+      <c r="Y64">
+        <f t="shared" si="6"/>
+        <v>6.5750950000000002E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>isotopes!A65</f>
         <v>Dy</v>
@@ -11476,24 +12163,24 @@
         <v>155.92427799999999</v>
       </c>
       <c r="D65">
-        <f>isotopes!D65</f>
-        <v>5.6000000000000001E-2</v>
+        <f>isotopes!D65/100</f>
+        <v>5.6000000000000006E-4</v>
       </c>
       <c r="E65">
         <f>IF(isotopes!E65-C65&lt;0,0,isotopes!E65-C65)</f>
         <v>2.0001270000000204</v>
       </c>
       <c r="F65">
-        <f>isotopes!F65</f>
-        <v>9.6000000000000002E-2</v>
+        <f>isotopes!F65/100</f>
+        <v>9.6000000000000002E-4</v>
       </c>
       <c r="G65">
         <f>IF(isotopes!G65-C65&lt;0,0,isotopes!G65-C65)</f>
         <v>4.0009160000000179</v>
       </c>
       <c r="H65">
-        <f>isotopes!H65</f>
-        <v>2.34</v>
+        <f>isotopes!H65/100</f>
+        <v>2.3399999999999997E-2</v>
       </c>
       <c r="I65">
         <f>isotopes!I65</f>
@@ -11531,8 +12218,22 @@
         <f>isotopes!Q65</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V65">
+        <v>391.10712702000001</v>
+      </c>
+      <c r="W65">
+        <f t="shared" si="7"/>
+        <v>3.0012667700000293</v>
+      </c>
+      <c r="X65">
+        <v>4.8751999999999997E-2</v>
+      </c>
+      <c r="Y65">
+        <f t="shared" si="6"/>
+        <v>4.8751999999999997E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>isotopes!A66</f>
         <v>Ho</v>
@@ -11546,15 +12247,15 @@
         <v>164.930319</v>
       </c>
       <c r="D66">
-        <f>isotopes!D66</f>
-        <v>100</v>
+        <f>isotopes!D66/100</f>
+        <v>1</v>
       </c>
       <c r="E66">
         <f>IF(isotopes!E66-C66&lt;0,0,isotopes!E66-C66)</f>
         <v>0</v>
       </c>
       <c r="F66">
-        <f>isotopes!F66</f>
+        <f>isotopes!F66/100</f>
         <v>0</v>
       </c>
       <c r="G66">
@@ -11562,7 +12263,7 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <f>isotopes!H66</f>
+        <f>isotopes!H66/100</f>
         <v>0</v>
       </c>
       <c r="I66">
@@ -11601,8 +12302,22 @@
         <f>isotopes!Q66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V66">
+        <v>391.10918687999998</v>
+      </c>
+      <c r="W66">
+        <f t="shared" si="7"/>
+        <v>3.0033266300000037</v>
+      </c>
+      <c r="X66">
+        <v>6.9918999999999995E-2</v>
+      </c>
+      <c r="Y66">
+        <f t="shared" si="6"/>
+        <v>6.9918999999999992E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>isotopes!A67</f>
         <v>Er</v>
@@ -11616,24 +12331,24 @@
         <v>161.928775</v>
       </c>
       <c r="D67">
-        <f>isotopes!D67</f>
-        <v>0.13700000000000001</v>
+        <f>isotopes!D67/100</f>
+        <v>1.3700000000000001E-3</v>
       </c>
       <c r="E67">
         <f>IF(isotopes!E67-C67&lt;0,0,isotopes!E67-C67)</f>
         <v>2.0004219999999862</v>
       </c>
       <c r="F67">
-        <f>isotopes!F67</f>
-        <v>1.609</v>
+        <f>isotopes!F67/100</f>
+        <v>1.609E-2</v>
       </c>
       <c r="G67">
         <f>IF(isotopes!G67-C67&lt;0,0,isotopes!G67-C67)</f>
         <v>4.0015150000000119</v>
       </c>
       <c r="H67">
-        <f>isotopes!H67</f>
-        <v>33.61</v>
+        <f>isotopes!H67/100</f>
+        <v>0.33610000000000001</v>
       </c>
       <c r="I67">
         <f>isotopes!I67</f>
@@ -11671,8 +12386,22 @@
         <f>isotopes!Q67</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V67">
+        <v>391.10960489000001</v>
+      </c>
+      <c r="W67">
+        <f t="shared" si="7"/>
+        <v>3.0037446400000363</v>
+      </c>
+      <c r="X67">
+        <v>2.1923999999999999E-2</v>
+      </c>
+      <c r="Y67">
+        <f t="shared" si="6"/>
+        <v>2.1923999999999999E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>isotopes!A68</f>
         <v>Tm</v>
@@ -11686,15 +12415,15 @@
         <v>168.934211</v>
       </c>
       <c r="D68">
-        <f>isotopes!D68</f>
-        <v>100</v>
+        <f>isotopes!D68/100</f>
+        <v>1</v>
       </c>
       <c r="E68">
         <f>IF(isotopes!E68-C68&lt;0,0,isotopes!E68-C68)</f>
         <v>0</v>
       </c>
       <c r="F68">
-        <f>isotopes!F68</f>
+        <f>isotopes!F68/100</f>
         <v>0</v>
       </c>
       <c r="G68">
@@ -11702,7 +12431,7 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <f>isotopes!H68</f>
+        <f>isotopes!H68/100</f>
         <v>0</v>
       </c>
       <c r="I68">
@@ -11741,8 +12470,22 @@
         <f>isotopes!Q68</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V68">
+        <v>391.11346086999998</v>
+      </c>
+      <c r="W68">
+        <f t="shared" si="7"/>
+        <v>3.0076006200000052</v>
+      </c>
+      <c r="X68">
+        <v>0.16891999999999999</v>
+      </c>
+      <c r="Y68">
+        <f t="shared" si="6"/>
+        <v>1.6891999999999999E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>isotopes!A69</f>
         <v>Yb</v>
@@ -11756,24 +12499,24 @@
         <v>167.93389400000001</v>
       </c>
       <c r="D69">
-        <f>isotopes!D69</f>
-        <v>0.127</v>
+        <f>isotopes!D69/100</f>
+        <v>1.2700000000000001E-3</v>
       </c>
       <c r="E69">
         <f>IF(isotopes!E69-C69&lt;0,0,isotopes!E69-C69)</f>
         <v>2.0008650000000046</v>
       </c>
       <c r="F69">
-        <f>isotopes!F69</f>
-        <v>3.04</v>
+        <f>isotopes!F69/100</f>
+        <v>3.04E-2</v>
       </c>
       <c r="G69">
         <f>IF(isotopes!G69-C69&lt;0,0,isotopes!G69-C69)</f>
         <v>3.0024279999999806</v>
       </c>
       <c r="H69">
-        <f>isotopes!H69</f>
-        <v>14.28</v>
+        <f>isotopes!H69/100</f>
+        <v>0.14279999999999998</v>
       </c>
       <c r="I69">
         <f>isotopes!I69</f>
@@ -11811,8 +12554,22 @@
         <f>isotopes!Q69</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V69">
+        <v>391.11592476999999</v>
+      </c>
+      <c r="W69">
+        <f t="shared" si="7"/>
+        <v>3.0100645200000145</v>
+      </c>
+      <c r="X69">
+        <v>0.1226</v>
+      </c>
+      <c r="Y69">
+        <f t="shared" si="6"/>
+        <v>1.2260000000000001E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>isotopes!A70</f>
         <v>Lu</v>
@@ -11826,23 +12583,23 @@
         <v>174.9407679</v>
       </c>
       <c r="D70">
-        <f>isotopes!D70</f>
-        <v>97.415999999999997</v>
+        <f>isotopes!D70/100</f>
+        <v>0.97415999999999991</v>
       </c>
       <c r="E70">
         <f>IF(isotopes!E70-C70&lt;0,0,isotopes!E70-C70)</f>
         <v>1.001914499999998</v>
       </c>
       <c r="F70">
-        <f>isotopes!F70</f>
-        <v>2.5840000000000001</v>
+        <f>isotopes!F70/100</f>
+        <v>2.5840000000000002E-2</v>
       </c>
       <c r="G70">
         <f>IF(isotopes!G70-C70&lt;0,0,isotopes!G70-C70)</f>
         <v>0</v>
       </c>
       <c r="H70">
-        <f>isotopes!H70</f>
+        <f>isotopes!H70/100</f>
         <v>0</v>
       </c>
       <c r="I70">
@@ -11881,8 +12638,22 @@
         <f>isotopes!Q70</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V70">
+        <v>392.10329994</v>
+      </c>
+      <c r="W70">
+        <f t="shared" si="7"/>
+        <v>3.9974396900000215</v>
+      </c>
+      <c r="X70">
+        <v>7.2062000000000001E-2</v>
+      </c>
+      <c r="Y70">
+        <f t="shared" si="6"/>
+        <v>7.2062000000000005E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>isotopes!A71</f>
         <v>Hf</v>
@@ -11896,24 +12667,24 @@
         <v>173.94004000000001</v>
       </c>
       <c r="D71">
-        <f>isotopes!D71</f>
-        <v>0.16200000000000001</v>
+        <f>isotopes!D71/100</f>
+        <v>1.6200000000000001E-3</v>
       </c>
       <c r="E71">
         <f>IF(isotopes!E71-C71&lt;0,0,isotopes!E71-C71)</f>
         <v>2.0013617999999838</v>
       </c>
       <c r="F71">
-        <f>isotopes!F71</f>
-        <v>5.2603999999999997</v>
+        <f>isotopes!F71/100</f>
+        <v>5.2603999999999998E-2</v>
       </c>
       <c r="G71">
         <f>IF(isotopes!G71-C71&lt;0,0,isotopes!G71-C71)</f>
         <v>3.0031799999999862</v>
       </c>
       <c r="H71">
-        <f>isotopes!H71</f>
-        <v>18.595300000000002</v>
+        <f>isotopes!H71/100</f>
+        <v>0.18595300000000001</v>
       </c>
       <c r="I71">
         <f>isotopes!I71</f>
@@ -11951,8 +12722,22 @@
         <f>isotopes!Q71</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V71">
+        <v>392.10715592000003</v>
+      </c>
+      <c r="W71">
+        <f t="shared" si="7"/>
+        <v>4.0012956700000473</v>
+      </c>
+      <c r="X71">
+        <v>0.26300400000000002</v>
+      </c>
+      <c r="Y71">
+        <f t="shared" si="6"/>
+        <v>2.6300400000000002E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>isotopes!A72</f>
         <v>Ta</v>
@@ -11966,23 +12751,23 @@
         <v>179.94746599999999</v>
       </c>
       <c r="D72">
-        <f>isotopes!D72</f>
-        <v>1.23E-2</v>
+        <f>isotopes!D72/100</f>
+        <v>1.2300000000000001E-4</v>
       </c>
       <c r="E72">
         <f>IF(isotopes!E72-C72&lt;0,0,isotopes!E72-C72)</f>
         <v>1.0005299999999977</v>
       </c>
       <c r="F72">
-        <f>isotopes!F72</f>
-        <v>99.987700000000004</v>
+        <f>isotopes!F72/100</f>
+        <v>0.99987700000000002</v>
       </c>
       <c r="G72">
         <f>IF(isotopes!G72-C72&lt;0,0,isotopes!G72-C72)</f>
         <v>0</v>
       </c>
       <c r="H72">
-        <f>isotopes!H72</f>
+        <f>isotopes!H72/100</f>
         <v>0</v>
       </c>
       <c r="I72">
@@ -12021,8 +12806,22 @@
         <f>isotopes!Q72</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V72">
+        <v>392.10961981999998</v>
+      </c>
+      <c r="W72">
+        <f t="shared" si="7"/>
+        <v>4.0037595699999997</v>
+      </c>
+      <c r="X72">
+        <v>0.64002999999999999</v>
+      </c>
+      <c r="Y72">
+        <f t="shared" si="6"/>
+        <v>6.4003000000000003E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>isotopes!A73</f>
         <v>W</v>
@@ -12036,24 +12835,24 @@
         <v>179.94670600000001</v>
       </c>
       <c r="D73">
-        <f>isotopes!D73</f>
-        <v>0.1198</v>
+        <f>isotopes!D73/100</f>
+        <v>1.1980000000000001E-3</v>
       </c>
       <c r="E73">
         <f>IF(isotopes!E73-C73&lt;0,0,isotopes!E73-C73)</f>
         <v>2.001499999999993</v>
       </c>
       <c r="F73">
-        <f>isotopes!F73</f>
-        <v>26.4985</v>
+        <f>isotopes!F73/100</f>
+        <v>0.26498500000000003</v>
       </c>
       <c r="G73">
         <f>IF(isotopes!G73-C73&lt;0,0,isotopes!G73-C73)</f>
         <v>3.0035184999999842</v>
       </c>
       <c r="H73">
-        <f>isotopes!H73</f>
-        <v>14.313599999999999</v>
+        <f>isotopes!H73/100</f>
+        <v>0.14313599999999999</v>
       </c>
       <c r="I73">
         <f>isotopes!I73</f>
@@ -12091,8 +12890,22 @@
         <f>isotopes!Q73</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V73">
+        <v>392.11048185999999</v>
+      </c>
+      <c r="W73">
+        <f t="shared" si="7"/>
+        <v>4.0046216100000152</v>
+      </c>
+      <c r="X73">
+        <v>1.0018000000000001E-2</v>
+      </c>
+      <c r="Y73">
+        <f t="shared" si="6"/>
+        <v>1.0018000000000001E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>isotopes!A74</f>
         <v>Re</v>
@@ -12106,23 +12919,23 @@
         <v>184.95295569999999</v>
       </c>
       <c r="D74">
-        <f>isotopes!D74</f>
-        <v>37.398000000000003</v>
+        <f>isotopes!D74/100</f>
+        <v>0.37398000000000003</v>
       </c>
       <c r="E74">
         <f>IF(isotopes!E74-C74&lt;0,0,isotopes!E74-C74)</f>
         <v>2.0027951000000144</v>
       </c>
       <c r="F74">
-        <f>isotopes!F74</f>
-        <v>62.601999999999997</v>
+        <f>isotopes!F74/100</f>
+        <v>0.62602000000000002</v>
       </c>
       <c r="G74">
         <f>IF(isotopes!G74-C74&lt;0,0,isotopes!G74-C74)</f>
         <v>0</v>
       </c>
       <c r="H74">
-        <f>isotopes!H74</f>
+        <f>isotopes!H74/100</f>
         <v>0</v>
       </c>
       <c r="I74">
@@ -12161,8 +12974,22 @@
         <f>isotopes!Q74</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V74">
+        <v>392.11254172000002</v>
+      </c>
+      <c r="W74">
+        <f t="shared" si="7"/>
+        <v>4.0066814700000464</v>
+      </c>
+      <c r="X74">
+        <v>1.4368000000000001E-2</v>
+      </c>
+      <c r="Y74">
+        <f t="shared" si="6"/>
+        <v>1.4368000000000001E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>isotopes!A75</f>
         <v>Os</v>
@@ -12176,24 +13003,24 @@
         <v>183.95249100000001</v>
       </c>
       <c r="D75">
-        <f>isotopes!D75</f>
-        <v>1.9699999999999999E-2</v>
+        <f>isotopes!D75/100</f>
+        <v>1.9699999999999999E-4</v>
       </c>
       <c r="E75">
         <f>IF(isotopes!E75-C75&lt;0,0,isotopes!E75-C75)</f>
         <v>2.0013469999999813</v>
       </c>
       <c r="F75">
-        <f>isotopes!F75</f>
-        <v>1.5859000000000001</v>
+        <f>isotopes!F75/100</f>
+        <v>1.5859000000000002E-2</v>
       </c>
       <c r="G75">
         <f>IF(isotopes!G75-C75&lt;0,0,isotopes!G75-C75)</f>
         <v>3.0032568999999967</v>
       </c>
       <c r="H75">
-        <f>isotopes!H75</f>
-        <v>1.9643999999999999</v>
+        <f>isotopes!H75/100</f>
+        <v>1.9643999999999998E-2</v>
       </c>
       <c r="I75">
         <f>isotopes!I75</f>
@@ -12231,8 +13058,22 @@
         <f>isotopes!Q75</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V75">
+        <v>392.11681571000003</v>
+      </c>
+      <c r="W75">
+        <f t="shared" si="7"/>
+        <v>4.0109554600000479</v>
+      </c>
+      <c r="X75">
+        <v>1.6442999999999999E-2</v>
+      </c>
+      <c r="Y75">
+        <f t="shared" si="6"/>
+        <v>1.6443E-4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>isotopes!A76</f>
         <v>Ir</v>
@@ -12246,23 +13087,23 @@
         <v>190.96059099999999</v>
       </c>
       <c r="D76">
-        <f>isotopes!D76</f>
-        <v>37.271999999999998</v>
+        <f>isotopes!D76/100</f>
+        <v>0.37272</v>
       </c>
       <c r="E76">
         <f>IF(isotopes!E76-C76&lt;0,0,isotopes!E76-C76)</f>
         <v>2.002332999999993</v>
       </c>
       <c r="F76">
-        <f>isotopes!F76</f>
-        <v>62.728000000000002</v>
+        <f>isotopes!F76/100</f>
+        <v>0.62728000000000006</v>
       </c>
       <c r="G76">
         <f>IF(isotopes!G76-C76&lt;0,0,isotopes!G76-C76)</f>
         <v>0</v>
       </c>
       <c r="H76">
-        <f>isotopes!H76</f>
+        <f>isotopes!H76/100</f>
         <v>0</v>
       </c>
       <c r="I76">
@@ -12301,8 +13142,22 @@
         <f>isotopes!Q76</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V76">
+        <v>393.11051076000001</v>
+      </c>
+      <c r="W76">
+        <f t="shared" si="7"/>
+        <v>5.0046505100000331</v>
+      </c>
+      <c r="X76">
+        <v>5.4046999999999998E-2</v>
+      </c>
+      <c r="Y76">
+        <f t="shared" si="6"/>
+        <v>5.4046999999999993E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>isotopes!A77</f>
         <v>Pt</v>
@@ -12316,24 +13171,24 @@
         <v>189.95993000000001</v>
       </c>
       <c r="D77">
-        <f>isotopes!D77</f>
-        <v>1.3634E-2</v>
+        <f>isotopes!D77/100</f>
+        <v>1.3634000000000001E-4</v>
       </c>
       <c r="E77">
         <f>IF(isotopes!E77-C77&lt;0,0,isotopes!E77-C77)</f>
         <v>2.0011049999999955</v>
       </c>
       <c r="F77">
-        <f>isotopes!F77</f>
-        <v>0.78265899999999999</v>
+        <f>isotopes!F77/100</f>
+        <v>7.8265899999999996E-3</v>
       </c>
       <c r="G77">
         <f>IF(isotopes!G77-C77&lt;0,0,isotopes!G77-C77)</f>
         <v>4.0027339999999754</v>
       </c>
       <c r="H77">
-        <f>isotopes!H77</f>
-        <v>32.966999999999999</v>
+        <f>isotopes!H77/100</f>
+        <v>0.32966999999999996</v>
       </c>
       <c r="I77">
         <f>isotopes!I77</f>
@@ -12371,8 +13226,22 @@
         <f>isotopes!Q77</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V77">
+        <v>393.11297466000002</v>
+      </c>
+      <c r="W77">
+        <f t="shared" si="7"/>
+        <v>5.0071144100000424</v>
+      </c>
+      <c r="X77">
+        <v>3.9226999999999998E-2</v>
+      </c>
+      <c r="Y77">
+        <f t="shared" si="6"/>
+        <v>3.9226999999999996E-4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>isotopes!A78</f>
         <v>Au</v>
@@ -12386,15 +13255,15 @@
         <v>196.96655200000001</v>
       </c>
       <c r="D78">
-        <f>isotopes!D78</f>
-        <v>100</v>
+        <f>isotopes!D78/100</f>
+        <v>1</v>
       </c>
       <c r="E78">
         <f>IF(isotopes!E78-C78&lt;0,0,isotopes!E78-C78)</f>
         <v>0</v>
       </c>
       <c r="F78">
-        <f>isotopes!F78</f>
+        <f>isotopes!F78/100</f>
         <v>0</v>
       </c>
       <c r="G78">
@@ -12402,7 +13271,7 @@
         <v>0</v>
       </c>
       <c r="H78">
-        <f>isotopes!H78</f>
+        <f>isotopes!H78/100</f>
         <v>0</v>
       </c>
       <c r="I78">
@@ -12442,7 +13311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>isotopes!A79</f>
         <v>Hg</v>
@@ -12456,24 +13325,24 @@
         <v>195.96581499999999</v>
       </c>
       <c r="D79">
-        <f>isotopes!D79</f>
-        <v>0.15343999999999999</v>
+        <f>isotopes!D79/100</f>
+        <v>1.5344E-3</v>
       </c>
       <c r="E79">
         <f>IF(isotopes!E79-C79&lt;0,0,isotopes!E79-C79)</f>
         <v>2.0009370000000217</v>
       </c>
       <c r="F79">
-        <f>isotopes!F79</f>
-        <v>9.968</v>
+        <f>isotopes!F79/100</f>
+        <v>9.9680000000000005E-2</v>
       </c>
       <c r="G79">
         <f>IF(isotopes!G79-C79&lt;0,0,isotopes!G79-C79)</f>
         <v>3.0024470000000179</v>
       </c>
       <c r="H79">
-        <f>isotopes!H79</f>
-        <v>16.873000000000001</v>
+        <f>isotopes!H79/100</f>
+        <v>0.16873000000000002</v>
       </c>
       <c r="I79">
         <f>isotopes!I79</f>
@@ -12512,7 +13381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>isotopes!A80</f>
         <v>Tl</v>
@@ -12526,23 +13395,23 @@
         <v>202.972329</v>
       </c>
       <c r="D80">
-        <f>isotopes!D80</f>
-        <v>29.524000000000001</v>
+        <f>isotopes!D80/100</f>
+        <v>0.29524</v>
       </c>
       <c r="E80">
         <f>IF(isotopes!E80-C80&lt;0,0,isotopes!E80-C80)</f>
         <v>2.0020829999999989</v>
       </c>
       <c r="F80">
-        <f>isotopes!F80</f>
-        <v>70.475999999999999</v>
+        <f>isotopes!F80/100</f>
+        <v>0.70475999999999994</v>
       </c>
       <c r="G80">
         <f>IF(isotopes!G80-C80&lt;0,0,isotopes!G80-C80)</f>
         <v>0</v>
       </c>
       <c r="H80">
-        <f>isotopes!H80</f>
+        <f>isotopes!H80/100</f>
         <v>0</v>
       </c>
       <c r="I80">
@@ -12596,24 +13465,24 @@
         <v>203.973029</v>
       </c>
       <c r="D81">
-        <f>isotopes!D81</f>
-        <v>1.4245000000000001</v>
+        <f>isotopes!D81/100</f>
+        <v>1.4245000000000001E-2</v>
       </c>
       <c r="E81">
         <f>IF(isotopes!E81-C81&lt;0,0,isotopes!E81-C81)</f>
         <v>2.001419999999996</v>
       </c>
       <c r="F81">
-        <f>isotopes!F81</f>
-        <v>24.1447</v>
+        <f>isotopes!F81/100</f>
+        <v>0.24144699999999999</v>
       </c>
       <c r="G81">
         <f>IF(isotopes!G81-C81&lt;0,0,isotopes!G81-C81)</f>
         <v>3.0028519999999901</v>
       </c>
       <c r="H81">
-        <f>isotopes!H81</f>
-        <v>22.082699999999999</v>
+        <f>isotopes!H81/100</f>
+        <v>0.220827</v>
       </c>
       <c r="I81">
         <f>isotopes!I81</f>
@@ -12666,15 +13535,15 @@
         <v>208.98038299999999</v>
       </c>
       <c r="D82">
-        <f>isotopes!D82</f>
-        <v>100</v>
+        <f>isotopes!D82/100</f>
+        <v>1</v>
       </c>
       <c r="E82">
         <f>IF(isotopes!E82-C82&lt;0,0,isotopes!E82-C82)</f>
         <v>0</v>
       </c>
       <c r="F82">
-        <f>isotopes!F82</f>
+        <f>isotopes!F82/100</f>
         <v>0</v>
       </c>
       <c r="G82">
@@ -12682,7 +13551,7 @@
         <v>0</v>
       </c>
       <c r="H82">
-        <f>isotopes!H82</f>
+        <f>isotopes!H82/100</f>
         <v>0</v>
       </c>
       <c r="I82">
@@ -12736,15 +13605,15 @@
         <v>232.0380504</v>
       </c>
       <c r="D83">
-        <f>isotopes!D83</f>
-        <v>100</v>
+        <f>isotopes!D83/100</f>
+        <v>1</v>
       </c>
       <c r="E83">
         <f>IF(isotopes!E83-C83&lt;0,0,isotopes!E83-C83)</f>
         <v>0</v>
       </c>
       <c r="F83">
-        <f>isotopes!F83</f>
+        <f>isotopes!F83/100</f>
         <v>0</v>
       </c>
       <c r="G83">
@@ -12752,7 +13621,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <f>isotopes!H83</f>
+        <f>isotopes!H83/100</f>
         <v>0</v>
       </c>
       <c r="I83">
@@ -12806,15 +13675,15 @@
         <v>231.0358789</v>
       </c>
       <c r="D84">
-        <f>isotopes!D84</f>
-        <v>100</v>
+        <f>isotopes!D84/100</f>
+        <v>1</v>
       </c>
       <c r="E84">
         <f>IF(isotopes!E84-C84&lt;0,0,isotopes!E84-C84)</f>
         <v>0</v>
       </c>
       <c r="F84">
-        <f>isotopes!F84</f>
+        <f>isotopes!F84/100</f>
         <v>0</v>
       </c>
       <c r="G84">
@@ -12822,7 +13691,7 @@
         <v>0</v>
       </c>
       <c r="H84">
-        <f>isotopes!H84</f>
+        <f>isotopes!H84/100</f>
         <v>0</v>
       </c>
       <c r="I84">
@@ -12876,24 +13745,24 @@
         <v>234.04094559999999</v>
       </c>
       <c r="D85">
-        <f>isotopes!D85</f>
-        <v>5.4799999999999996E-3</v>
+        <f>isotopes!D85/100</f>
+        <v>5.4799999999999997E-5</v>
       </c>
       <c r="E85">
         <f>IF(isotopes!E85-C85&lt;0,0,isotopes!E85-C85)</f>
         <v>1.0029775000000143</v>
       </c>
       <c r="F85">
-        <f>isotopes!F85</f>
-        <v>0.72</v>
+        <f>isotopes!F85/100</f>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="G85">
         <f>IF(isotopes!G85-C85&lt;0,0,isotopes!G85-C85)</f>
         <v>4.0098370000000045</v>
       </c>
       <c r="H85">
-        <f>isotopes!H85</f>
-        <v>99.274500000000003</v>
+        <f>isotopes!H85/100</f>
+        <v>0.99274499999999999</v>
       </c>
       <c r="I85">
         <f>isotopes!I85</f>

</xml_diff>